<commit_message>
Se suben las actlizaciones de la semana 23/09/22
</commit_message>
<xml_diff>
--- a/MonitorRMA/BaseDatos/Estructura.xlsx
+++ b/MonitorRMA/BaseDatos/Estructura.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DatosPersonales\Personales\Repositorio\GitHub\DesarrolloARM\MonitorRMA\BaseDatos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{209CABD1-A603-44E0-A670-6C5AEC29BEE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30425FBC-424E-4786-93C2-88188E7D5DB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="1" xr2:uid="{010BB1C2-CC3F-48D4-9CA6-4C5256A0A30C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="10845" activeTab="1" xr2:uid="{010BB1C2-CC3F-48D4-9CA6-4C5256A0A30C}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja2" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="187">
   <si>
     <t>RMA</t>
   </si>
@@ -568,6 +568,36 @@
   </si>
   <si>
     <t>oEFPCa1Z1k+qV2t65a98yA==</t>
+  </si>
+  <si>
+    <t>FORMA R15</t>
+  </si>
+  <si>
+    <t>CONTABILIDAD NEPE</t>
+  </si>
+  <si>
+    <t>VALIDADOR DE INTERESES</t>
+  </si>
+  <si>
+    <t>VALIDADOR DE FIDEICOMISOS</t>
+  </si>
+  <si>
+    <t>FORMA 35 DECLARACION INFORMATIVA</t>
+  </si>
+  <si>
+    <t>dyp_pp_forma_r15</t>
+  </si>
+  <si>
+    <t>rc_contabilidad_nepe</t>
+  </si>
+  <si>
+    <t>dyp_lda_validador_de_intereses</t>
+  </si>
+  <si>
+    <t>dyp_lda_validador_de_fideicomisos</t>
+  </si>
+  <si>
+    <t>dyp_pp_forma_35</t>
   </si>
 </sst>
 </file>
@@ -944,10 +974,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08A8E975-DFF4-4A8E-97A2-75F45BA0815F}">
-  <dimension ref="A1:K93"/>
+  <dimension ref="A1:K95"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="A22" sqref="A22:A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -978,7 +1008,7 @@
         <v>CREATE TABLE Tablas(</v>
       </c>
       <c r="J1" s="1" t="str">
-        <f t="shared" ref="J1:J64" si="1">IF(I1="",_xlfn.CONCAT("	", A1," ",B1,IF(C1&gt;0,_xlfn.CONCAT("(",C1,")"),""),IF(D1=1," NOT NULL"," NULL"),IF(F1=1," IDENTITY(1,1)",""),IF(E1=1," PRIMARY KEY",""),IF(G1&lt;&gt;"",_xlfn.CONCAT(" ",G1),""),IF(I2=0,")
+        <f t="shared" ref="J1:J66" si="1">IF(I1="",_xlfn.CONCAT("	", A1," ",B1,IF(C1&gt;0,_xlfn.CONCAT("(",C1,")"),""),IF(D1=1," NOT NULL"," NULL"),IF(F1=1," IDENTITY(1,1)",""),IF(E1=1," PRIMARY KEY",""),IF(G1&lt;&gt;"",_xlfn.CONCAT(" ",G1),""),IF(I2=0,")
 GO",", ")),IF(I1=1,_xlfn.CONCAT(B1,", "), ""))</f>
         <v/>
       </c>
@@ -1011,7 +1041,7 @@
       </c>
       <c r="H2" s="3"/>
       <c r="I2" s="1">
-        <f t="shared" ref="I2:I18" si="2">IF(A2="", IF(C2="", IF(B2="",0,1), _xlfn.CONCAT("CREATE TABLE ",C2,"(")), IF(A2="CAMPO", 0, ""))</f>
+        <f t="shared" ref="I2:I65" si="2">IF(A2="", IF(C2="", IF(B2="",0,1), _xlfn.CONCAT("CREATE TABLE ",C2,"(")), IF(A2="CAMPO", 0, ""))</f>
         <v>0</v>
       </c>
       <c r="J2" s="1" t="str">
@@ -1019,7 +1049,7 @@
         <v/>
       </c>
       <c r="K2" s="1" t="str">
-        <f t="shared" ref="K2:K18" si="3">IF(I2=0, "", IF(J2="", I2, J2))</f>
+        <f t="shared" ref="K2:K65" si="3">IF(I2=0, "", IF(J2="", I2, J2))</f>
         <v/>
       </c>
     </row>
@@ -1428,7 +1458,7 @@
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="I19" s="1" t="str">
-        <f t="shared" ref="I19:I82" si="4">IF(A19="", IF(C19="", IF(B19="",0,1), _xlfn.CONCAT("CREATE TABLE ",C19,"(")), IF(A19="CAMPO", 0, ""))</f>
+        <f t="shared" si="2"/>
         <v>CREATE TABLE Empleados(</v>
       </c>
       <c r="J19" s="1" t="str">
@@ -1436,7 +1466,7 @@
         <v/>
       </c>
       <c r="K19" s="1" t="str">
-        <f t="shared" ref="K19:K82" si="5">IF(I19=0, "", IF(J19="", I19, J19))</f>
+        <f t="shared" si="3"/>
         <v>CREATE TABLE Empleados(</v>
       </c>
     </row>
@@ -1463,7 +1493,7 @@
         <v>21</v>
       </c>
       <c r="I20" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J20" s="1" t="str">
@@ -1471,7 +1501,7 @@
         <v/>
       </c>
       <c r="K20" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -1495,696 +1525,698 @@
         <v>1</v>
       </c>
       <c r="I21" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="J21" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(I21="",_xlfn.CONCAT("	", A21," ",B21,IF(C21&gt;0,_xlfn.CONCAT("(",C21,")"),""),IF(D21=1," NOT NULL"," NULL"),IF(F21=1," IDENTITY(1,1)",""),IF(E21=1," PRIMARY KEY",""),IF(G21&lt;&gt;"",_xlfn.CONCAT(" ",G21),""),IF(I24=0,")
+GO",", ")),IF(I21=1,_xlfn.CONCAT(B21,", "), ""))</f>
         <v xml:space="preserve">	nIdEmpleado INT NOT NULL IDENTITY(1,1) PRIMARY KEY, </v>
       </c>
       <c r="K21" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">	nIdEmpleado INT NOT NULL IDENTITY(1,1) PRIMARY KEY, </v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>5</v>
+      <c r="A22" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>3</v>
       </c>
       <c r="C22" s="4">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="D22" s="4">
-        <v>1</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
       <c r="I22" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="J22" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">	sNombre nVarChar(150) NOT NULL, </v>
+        <f t="shared" ref="J22:J85" si="4">IF(I22="",_xlfn.CONCAT("	", A22," ",B22,IF(C22&gt;0,_xlfn.CONCAT("(",C22,")"),""),IF(D22=1," NOT NULL"," NULL"),IF(F22=1," IDENTITY(1,1)",""),IF(E22=1," PRIMARY KEY",""),IF(G22&lt;&gt;"",_xlfn.CONCAT(" ",G22),""),IF(I25=0,")
+GO",", ")),IF(I22=1,_xlfn.CONCAT(B22,", "), ""))</f>
+        <v xml:space="preserve">	nIdArea INT NULL, </v>
       </c>
       <c r="K22" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">	sNombre nVarChar(150) NOT NULL, </v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">	nIdArea INT NULL, </v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>5</v>
+      <c r="A23" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>3</v>
       </c>
       <c r="C23" s="4">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="D23" s="4">
-        <v>1</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
       <c r="I23" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="J23" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">	sApellido1 nVarChar(100) NOT NULL, </v>
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">	nIdAplicativo INT NULL, </v>
       </c>
       <c r="K23" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">	sApellido1 nVarChar(100) NOT NULL, </v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">	nIdAplicativo INT NULL, </v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C24" s="4">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="D24" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I24" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="J24" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">	sApellido2 nVarChar(100) NULL, </v>
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">	sNombre nVarChar(150) NOT NULL, </v>
       </c>
       <c r="K24" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">	sApellido2 nVarChar(100) NULL, </v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">	sNombre nVarChar(150) NOT NULL, </v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C25" s="4">
-        <v>50</v>
-      </c>
-      <c r="D25" s="1">
+        <v>100</v>
+      </c>
+      <c r="D25" s="4">
         <v>1</v>
       </c>
       <c r="I25" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="J25" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">	sUsuario nVarChar(50) NOT NULL, </v>
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">	sApellido1 nVarChar(100) NOT NULL, </v>
       </c>
       <c r="K25" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">	sUsuario nVarChar(50) NOT NULL, </v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">	sApellido1 nVarChar(100) NOT NULL, </v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C26" s="4">
-        <v>150</v>
-      </c>
-      <c r="D26" s="1">
-        <v>1</v>
+        <v>100</v>
+      </c>
+      <c r="D26" s="4">
+        <v>0</v>
       </c>
       <c r="I26" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="J26" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">	sContra nVarChar(150) NOT NULL, </v>
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">	sApellido2 nVarChar(100) NULL, </v>
       </c>
       <c r="K26" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">	sContra nVarChar(150) NOT NULL, </v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">	sApellido2 nVarChar(100) NULL, </v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>45</v>
+        <v>141</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C27" s="4">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="D27" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I27" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="J27" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">	Orden INT NULL, </v>
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">	sUsuario nVarChar(50) NOT NULL, </v>
       </c>
       <c r="K27" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">	Orden INT NULL, </v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">	sUsuario nVarChar(50) NOT NULL, </v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>47</v>
+        <v>5</v>
       </c>
       <c r="C28" s="4">
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="D28" s="1">
         <v>1</v>
       </c>
       <c r="I28" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="J28" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">	Root Bit NOT NULL, </v>
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">	sContra nVarChar(150) NOT NULL, </v>
       </c>
       <c r="K28" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">	Root Bit NOT NULL, </v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">	sContra nVarChar(150) NOT NULL, </v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C29" s="4">
+        <v>0</v>
+      </c>
+      <c r="D29" s="1">
+        <v>0</v>
+      </c>
+      <c r="I29" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="J29" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">	Orden INT NULL, </v>
+      </c>
+      <c r="K29" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">	Orden INT NULL, </v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C30" s="4">
+        <v>0</v>
+      </c>
+      <c r="D30" s="1">
+        <v>1</v>
+      </c>
+      <c r="I30" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="J30" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">	Root Bit NOT NULL, </v>
+      </c>
+      <c r="K30" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">	Root Bit NOT NULL, </v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B31" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C29" s="4">
-        <v>0</v>
-      </c>
-      <c r="D29" s="1">
-        <v>1</v>
-      </c>
-      <c r="I29" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="J29" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">	Estado Bit NOT NULL, </v>
-      </c>
-      <c r="K29" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">	Estado Bit NOT NULL, </v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B30" s="2" t="str">
-        <f>_xlfn.CONCAT("	CONSTRAINT AK_", $C$19, "_NombreEmpleado  UNIQUE (",$A$22,", ",$A$23,", ",$A$24,")")</f>
+      <c r="C31" s="4">
+        <v>0</v>
+      </c>
+      <c r="D31" s="1">
+        <v>1</v>
+      </c>
+      <c r="I31" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="J31" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">	Estado Bit NOT NULL)
+GO</v>
+      </c>
+      <c r="K31" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">	Estado Bit NOT NULL)
+GO</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B32" s="2" t="str">
+        <f>_xlfn.CONCAT("	CONSTRAINT AK_", $C$19, "_NombreEmpleado  UNIQUE (",$A$24,", ",$A$25,", ",$A$26,")")</f>
         <v xml:space="preserve">	CONSTRAINT AK_Empleados_NombreEmpleado  UNIQUE (sNombre, sApellido1, sApellido2)</v>
       </c>
-      <c r="I30" s="1">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="J30" s="1" t="str">
-        <f t="shared" si="1"/>
+      <c r="I32" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J32" s="1" t="str">
+        <f t="shared" si="4"/>
         <v xml:space="preserve">	CONSTRAINT AK_Empleados_NombreEmpleado  UNIQUE (sNombre, sApellido1, sApellido2), </v>
       </c>
-      <c r="K30" s="1" t="str">
-        <f t="shared" si="5"/>
+      <c r="K32" s="1" t="str">
+        <f t="shared" si="3"/>
         <v xml:space="preserve">	CONSTRAINT AK_Empleados_NombreEmpleado  UNIQUE (sNombre, sApellido1, sApellido2), </v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B31" s="2" t="str">
-        <f>_xlfn.CONCAT("	CONSTRAINT AK_", $C$19, "_Usuario  UNIQUE (",$A$25,")")</f>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B33" s="2" t="str">
+        <f>_xlfn.CONCAT("	CONSTRAINT AK_", $C$19, "_Usuario  UNIQUE (",$A$27,")")</f>
         <v xml:space="preserve">	CONSTRAINT AK_Empleados_Usuario  UNIQUE (sUsuario)</v>
       </c>
-      <c r="I31" s="1">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="J31" s="1" t="str">
-        <f t="shared" si="1"/>
+      <c r="I33" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J33" s="1" t="str">
+        <f t="shared" si="4"/>
         <v xml:space="preserve">	CONSTRAINT AK_Empleados_Usuario  UNIQUE (sUsuario), </v>
       </c>
-      <c r="K31" s="1" t="str">
-        <f t="shared" si="5"/>
+      <c r="K33" s="1" t="str">
+        <f t="shared" si="3"/>
         <v xml:space="preserve">	CONSTRAINT AK_Empleados_Usuario  UNIQUE (sUsuario), </v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C32" s="4"/>
-      <c r="I32" s="1">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="J32" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="K32" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C33" s="4" t="s">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C34" s="4"/>
+      <c r="I34" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J34" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="K34" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C35" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="I33" s="1" t="str">
-        <f t="shared" si="4"/>
+      <c r="I35" s="1" t="str">
+        <f t="shared" si="2"/>
         <v>CREATE TABLE EmpleadoArea(</v>
       </c>
-      <c r="J33" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="K33" s="1" t="str">
-        <f t="shared" si="5"/>
+      <c r="J35" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="K35" s="1" t="str">
+        <f t="shared" si="3"/>
         <v>CREATE TABLE EmpleadoArea(</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A34" s="3" t="s">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A36" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="B36" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="C36" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D34" s="3" t="s">
+      <c r="D36" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E34" s="3" t="s">
+      <c r="E36" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F34" s="3" t="s">
+      <c r="F36" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G34" s="3" t="s">
+      <c r="G36" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="I34" s="1">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="J34" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="K34" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A35" s="2" t="s">
+      <c r="I36" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J36" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="K36" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A37" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B37" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C35" s="4">
-        <v>0</v>
-      </c>
-      <c r="D35" s="4">
-        <v>1</v>
-      </c>
-      <c r="E35" s="4"/>
-      <c r="F35" s="4"/>
-      <c r="G35" s="1" t="str">
+      <c r="C37" s="4">
+        <v>0</v>
+      </c>
+      <c r="D37" s="4">
+        <v>1</v>
+      </c>
+      <c r="E37" s="4"/>
+      <c r="F37" s="4"/>
+      <c r="G37" s="1" t="str">
         <f>_xlfn.CONCAT("REFERENCES ", $C$19, "(", $A$21, ")")</f>
         <v>REFERENCES Empleados(nIdEmpleado)</v>
       </c>
-      <c r="I35" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="J35" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">	nIdEmpleado INT NOT NULL REFERENCES Empleados(nIdEmpleado), </v>
-      </c>
-      <c r="K35" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">	nIdEmpleado INT NOT NULL REFERENCES Empleados(nIdEmpleado), </v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A36" s="1" t="s">
+      <c r="I37" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="J37" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">	nIdEmpleado INT NOT NULL REFERENCES Empleados(nIdEmpleado))
+GO</v>
+      </c>
+      <c r="K37" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">	nIdEmpleado INT NOT NULL REFERENCES Empleados(nIdEmpleado))
+GO</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B38" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C36" s="4">
-        <v>0</v>
-      </c>
-      <c r="D36" s="4">
-        <v>1</v>
-      </c>
-      <c r="G36" s="1" t="str">
+      <c r="C38" s="4">
+        <v>0</v>
+      </c>
+      <c r="D38" s="4">
+        <v>1</v>
+      </c>
+      <c r="G38" s="1" t="str">
         <f>_xlfn.CONCAT("REFERENCES ", $C$8, "(", $A$10, ")")</f>
         <v>REFERENCES TablasDetalles(nIdTablaDetalle)</v>
       </c>
-      <c r="I36" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="J36" s="1" t="str">
-        <f t="shared" si="1"/>
+      <c r="I38" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="J38" s="1" t="str">
+        <f t="shared" si="4"/>
         <v xml:space="preserve">	nIdArea INT NOT NULL REFERENCES TablasDetalles(nIdTablaDetalle), </v>
       </c>
-      <c r="K36" s="1" t="str">
-        <f t="shared" si="5"/>
+      <c r="K38" s="1" t="str">
+        <f t="shared" si="3"/>
         <v xml:space="preserve">	nIdArea INT NOT NULL REFERENCES TablasDetalles(nIdTablaDetalle), </v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B37" s="2" t="str">
-        <f>_xlfn.CONCAT("	CONSTRAINT AK_", $C$33, "  UNIQUE (",$A$35,", ",$A$36,")")</f>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B39" s="2" t="str">
+        <f>_xlfn.CONCAT("	CONSTRAINT AK_", $C$35, "  UNIQUE (",$A$37,", ",$A$38,")")</f>
         <v xml:space="preserve">	CONSTRAINT AK_EmpleadoArea  UNIQUE (nIdEmpleado, nIdArea)</v>
       </c>
-      <c r="C37" s="4"/>
-      <c r="D37" s="4"/>
-      <c r="I37" s="1">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="J37" s="1" t="str">
-        <f t="shared" si="1"/>
+      <c r="C39" s="4"/>
+      <c r="D39" s="4"/>
+      <c r="I39" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J39" s="1" t="str">
+        <f t="shared" si="4"/>
         <v xml:space="preserve">	CONSTRAINT AK_EmpleadoArea  UNIQUE (nIdEmpleado, nIdArea), </v>
       </c>
-      <c r="K37" s="1" t="str">
-        <f t="shared" si="5"/>
+      <c r="K39" s="1" t="str">
+        <f t="shared" si="3"/>
         <v xml:space="preserve">	CONSTRAINT AK_EmpleadoArea  UNIQUE (nIdEmpleado, nIdArea), </v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C38" s="4"/>
-      <c r="D38" s="4"/>
-      <c r="I38" s="1">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="J38" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="K38" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C39" s="4" t="s">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C40" s="4"/>
+      <c r="D40" s="4"/>
+      <c r="I40" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J40" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="K40" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C41" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="D39" s="4"/>
-      <c r="I39" s="1" t="str">
-        <f t="shared" si="4"/>
+      <c r="D41" s="4"/>
+      <c r="I41" s="1" t="str">
+        <f t="shared" si="2"/>
         <v>CREATE TABLE AreaAplicativo(</v>
       </c>
-      <c r="J39" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="K39" s="1" t="str">
-        <f t="shared" si="5"/>
+      <c r="J41" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="K41" s="1" t="str">
+        <f t="shared" si="3"/>
         <v>CREATE TABLE AreaAplicativo(</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A40" s="3" t="s">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A42" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B40" s="3" t="s">
+      <c r="B42" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C40" s="3" t="s">
+      <c r="C42" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D40" s="3" t="s">
+      <c r="D42" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E40" s="3" t="s">
+      <c r="E42" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F40" s="3" t="s">
+      <c r="F42" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G40" s="3" t="s">
+      <c r="G42" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="I40" s="1">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="J40" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="K40" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A41" s="2" t="s">
+      <c r="I42" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J42" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="K42" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A43" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="B43" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C41" s="4">
-        <v>0</v>
-      </c>
-      <c r="D41" s="4">
-        <v>1</v>
-      </c>
-      <c r="E41" s="4"/>
-      <c r="F41" s="4"/>
-      <c r="G41" s="1" t="str">
+      <c r="C43" s="4">
+        <v>0</v>
+      </c>
+      <c r="D43" s="4">
+        <v>1</v>
+      </c>
+      <c r="E43" s="4"/>
+      <c r="F43" s="4"/>
+      <c r="G43" s="1" t="str">
         <f>_xlfn.CONCAT("REFERENCES ", $C$8, "(", $A$10, ")")</f>
         <v>REFERENCES TablasDetalles(nIdTablaDetalle)</v>
       </c>
-      <c r="I41" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="J41" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">	nIdArea INT NOT NULL REFERENCES TablasDetalles(nIdTablaDetalle), </v>
-      </c>
-      <c r="K41" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">	nIdArea INT NOT NULL REFERENCES TablasDetalles(nIdTablaDetalle), </v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A42" s="1" t="s">
+      <c r="I43" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="J43" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">	nIdArea INT NOT NULL REFERENCES TablasDetalles(nIdTablaDetalle))
+GO</v>
+      </c>
+      <c r="K43" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">	nIdArea INT NOT NULL REFERENCES TablasDetalles(nIdTablaDetalle))
+GO</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B44" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C42" s="4">
-        <v>0</v>
-      </c>
-      <c r="D42" s="4">
-        <v>1</v>
-      </c>
-      <c r="G42" s="1" t="str">
+      <c r="C44" s="4">
+        <v>0</v>
+      </c>
+      <c r="D44" s="4">
+        <v>1</v>
+      </c>
+      <c r="G44" s="1" t="str">
         <f>_xlfn.CONCAT("REFERENCES ", $C$8, "(", $A$10, ")")</f>
         <v>REFERENCES TablasDetalles(nIdTablaDetalle)</v>
       </c>
-      <c r="I42" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="J42" s="1" t="str">
-        <f t="shared" si="1"/>
+      <c r="I44" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="J44" s="1" t="str">
+        <f t="shared" si="4"/>
         <v xml:space="preserve">	nIdAplicativo INT NOT NULL REFERENCES TablasDetalles(nIdTablaDetalle), </v>
       </c>
-      <c r="K42" s="1" t="str">
-        <f t="shared" si="5"/>
+      <c r="K44" s="1" t="str">
+        <f t="shared" si="3"/>
         <v xml:space="preserve">	nIdAplicativo INT NOT NULL REFERENCES TablasDetalles(nIdTablaDetalle), </v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B43" s="2" t="str">
-        <f>_xlfn.CONCAT("	CONSTRAINT AK_", $C$39, "  UNIQUE (",$A$41,", ",$A$42,")")</f>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B45" s="2" t="str">
+        <f>_xlfn.CONCAT("	CONSTRAINT AK_", $C$41, "  UNIQUE (",$A$43,", ",$A$44,")")</f>
         <v xml:space="preserve">	CONSTRAINT AK_AreaAplicativo  UNIQUE (nIdArea, nIdAplicativo)</v>
       </c>
-      <c r="C43" s="4"/>
-      <c r="D43" s="4"/>
-      <c r="I43" s="1">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="J43" s="1" t="str">
-        <f t="shared" si="1"/>
+      <c r="C45" s="4"/>
+      <c r="D45" s="4"/>
+      <c r="I45" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J45" s="1" t="str">
+        <f t="shared" si="4"/>
         <v xml:space="preserve">	CONSTRAINT AK_AreaAplicativo  UNIQUE (nIdArea, nIdAplicativo), </v>
       </c>
-      <c r="K43" s="1" t="str">
-        <f t="shared" si="5"/>
+      <c r="K45" s="1" t="str">
+        <f t="shared" si="3"/>
         <v xml:space="preserve">	CONSTRAINT AK_AreaAplicativo  UNIQUE (nIdArea, nIdAplicativo), </v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="I44" s="1">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="J44" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="K44" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C45" s="2" t="s">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I46" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J46" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="K46" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C47" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D45" s="2"/>
-      <c r="E45" s="2"/>
-      <c r="I45" s="1" t="str">
-        <f t="shared" si="4"/>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2"/>
+      <c r="I47" s="1" t="str">
+        <f t="shared" si="2"/>
         <v>CREATE TABLE DatosReqs(</v>
       </c>
-      <c r="J45" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="K45" s="1" t="str">
-        <f t="shared" si="5"/>
+      <c r="J47" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="K47" s="1" t="str">
+        <f t="shared" si="3"/>
         <v>CREATE TABLE DatosReqs(</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A46" s="3" t="s">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A48" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B46" s="3" t="s">
+      <c r="B48" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C46" s="3" t="s">
+      <c r="C48" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D46" s="3" t="s">
+      <c r="D48" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E46" s="3" t="s">
+      <c r="E48" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F46" s="3" t="s">
+      <c r="F48" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G46" s="3" t="s">
+      <c r="G48" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="H46" s="3"/>
-      <c r="I46" s="1">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="J46" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="K46" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A47" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C47" s="1">
-        <v>0</v>
-      </c>
-      <c r="D47" s="1">
-        <v>1</v>
-      </c>
-      <c r="E47" s="1">
-        <v>1</v>
-      </c>
-      <c r="F47" s="1">
-        <v>1</v>
-      </c>
-      <c r="I47" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="J47" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">	nIdRequerimiento INT NOT NULL IDENTITY(1,1) PRIMARY KEY, </v>
-      </c>
-      <c r="K47" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">	nIdRequerimiento INT NOT NULL IDENTITY(1,1) PRIMARY KEY, </v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A48" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C48" s="1">
-        <v>0</v>
-      </c>
-      <c r="D48" s="1">
-        <v>1</v>
-      </c>
-      <c r="G48" s="1" t="str">
-        <f>_xlfn.CONCAT("REFERENCES ", $C$8, "(", $A$10, ")")</f>
-        <v>REFERENCES TablasDetalles(nIdTablaDetalle)</v>
-      </c>
-      <c r="I48" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v/>
+      <c r="H48" s="3"/>
+      <c r="I48" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
       <c r="J48" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">	nIdTipoRequerimiento INT NOT NULL REFERENCES TablasDetalles(nIdTablaDetalle), </v>
+        <f t="shared" si="4"/>
+        <v/>
       </c>
       <c r="K48" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">	nIdTipoRequerimiento INT NOT NULL REFERENCES TablasDetalles(nIdTablaDetalle), </v>
+        <f t="shared" si="3"/>
+        <v/>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>39</v>
+        <v>2</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>3</v>
@@ -2195,26 +2227,28 @@
       <c r="D49" s="1">
         <v>1</v>
       </c>
-      <c r="G49" s="1" t="str">
-        <f>_xlfn.CONCAT("REFERENCES ", $C$8, "(", $A$10, ")")</f>
-        <v>REFERENCES TablasDetalles(nIdTablaDetalle)</v>
+      <c r="E49" s="1">
+        <v>1</v>
+      </c>
+      <c r="F49" s="1">
+        <v>1</v>
       </c>
       <c r="I49" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="J49" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">	nIdEstado INT NOT NULL REFERENCES TablasDetalles(nIdTablaDetalle), </v>
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">	nIdRequerimiento INT NOT NULL IDENTITY(1,1) PRIMARY KEY, </v>
       </c>
       <c r="K49" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">	nIdEstado INT NOT NULL REFERENCES TablasDetalles(nIdTablaDetalle), </v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">	nIdRequerimiento INT NOT NULL IDENTITY(1,1) PRIMARY KEY, </v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>43</v>
+        <v>11</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>3</v>
@@ -2230,21 +2264,21 @@
         <v>REFERENCES TablasDetalles(nIdTablaDetalle)</v>
       </c>
       <c r="I50" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="J50" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">	nIdResponsable INT NOT NULL REFERENCES TablasDetalles(nIdTablaDetalle), </v>
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">	nIdTipoRequerimiento INT NOT NULL REFERENCES TablasDetalles(nIdTablaDetalle), </v>
       </c>
       <c r="K50" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">	nIdResponsable INT NOT NULL REFERENCES TablasDetalles(nIdTablaDetalle), </v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">	nIdTipoRequerimiento INT NOT NULL REFERENCES TablasDetalles(nIdTablaDetalle), </v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>118</v>
+        <v>39</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>3</v>
@@ -2260,151 +2294,159 @@
         <v>REFERENCES TablasDetalles(nIdTablaDetalle)</v>
       </c>
       <c r="I51" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="J51" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">	nIdAplicativo INT NOT NULL REFERENCES TablasDetalles(nIdTablaDetalle), </v>
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">	nIdEstado INT NOT NULL REFERENCES TablasDetalles(nIdTablaDetalle), </v>
       </c>
       <c r="K51" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">	nIdAplicativo INT NOT NULL REFERENCES TablasDetalles(nIdTablaDetalle), </v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">	nIdEstado INT NOT NULL REFERENCES TablasDetalles(nIdTablaDetalle), </v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>6</v>
+        <v>43</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C52" s="1">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="D52" s="1">
         <v>1</v>
       </c>
+      <c r="G52" s="1" t="str">
+        <f>_xlfn.CONCAT("REFERENCES ", $C$8, "(", $A$10, ")")</f>
+        <v>REFERENCES TablasDetalles(nIdTablaDetalle)</v>
+      </c>
       <c r="I52" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="J52" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">	Requerimiento nVarChar(20) NOT NULL, </v>
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">	nIdResponsable INT NOT NULL REFERENCES TablasDetalles(nIdTablaDetalle), </v>
       </c>
       <c r="K52" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">	Requerimiento nVarChar(20) NOT NULL, </v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">	nIdResponsable INT NOT NULL REFERENCES TablasDetalles(nIdTablaDetalle), </v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>12</v>
+        <v>118</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C53" s="1">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="D53" s="1">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="G53" s="1" t="str">
+        <f>_xlfn.CONCAT("REFERENCES ", $C$8, "(", $A$10, ")")</f>
+        <v>REFERENCES TablasDetalles(nIdTablaDetalle)</v>
       </c>
       <c r="I53" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="J53" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">	REQS nVarChar(20) NULL, </v>
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">	nIdAplicativo INT NOT NULL REFERENCES TablasDetalles(nIdTablaDetalle), </v>
       </c>
       <c r="K53" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">	REQS nVarChar(20) NULL, </v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">	nIdAplicativo INT NOT NULL REFERENCES TablasDetalles(nIdTablaDetalle), </v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C54" s="1">
-        <v>250</v>
+        <v>20</v>
       </c>
       <c r="D54" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I54" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="J54" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">	Titulo nVarChar(250) NULL, </v>
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">	Requerimiento nVarChar(20) NOT NULL, </v>
       </c>
       <c r="K54" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">	Titulo nVarChar(250) NULL, </v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">	Requerimiento nVarChar(20) NOT NULL, </v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C55" s="1">
-        <v>350</v>
+        <v>20</v>
       </c>
       <c r="D55" s="1">
         <v>0</v>
       </c>
       <c r="I55" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="J55" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">	Resumen nVarChar(350) NULL, </v>
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">	REQS nVarChar(20) NULL, </v>
       </c>
       <c r="K55" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">	Resumen nVarChar(350) NULL, </v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">	REQS nVarChar(20) NULL, </v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C56" s="1">
-        <v>15</v>
+        <v>250</v>
       </c>
       <c r="D56" s="1">
         <v>0</v>
       </c>
       <c r="I56" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="J56" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">	RFC nChar(15) NULL, </v>
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">	Titulo nVarChar(250) NULL, </v>
       </c>
       <c r="K56" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">	RFC nChar(15) NULL, </v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">	Titulo nVarChar(250) NULL, </v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>48</v>
+        <v>18</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>5</v>
@@ -2416,915 +2458,977 @@
         <v>0</v>
       </c>
       <c r="I57" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="J57" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">	IdentificadorReq nVarChar(350) NULL, </v>
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">	Resumen nVarChar(350) NULL, </v>
       </c>
       <c r="K57" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">	IdentificadorReq nVarChar(350) NULL, </v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">	Resumen nVarChar(350) NULL, </v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>126</v>
+        <v>1</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>55</v>
+        <v>4</v>
       </c>
       <c r="C58" s="1">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="D58" s="1">
         <v>0</v>
       </c>
       <c r="I58" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="J58" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">	FechaRecepcion DateTime NULL, </v>
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">	RFC nChar(15) NULL, </v>
       </c>
       <c r="K58" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">	FechaRecepcion DateTime NULL, </v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">	RFC nChar(15) NULL, </v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>127</v>
+        <v>48</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>55</v>
+        <v>5</v>
       </c>
       <c r="C59" s="1">
-        <v>0</v>
+        <v>350</v>
       </c>
       <c r="D59" s="1">
         <v>0</v>
       </c>
       <c r="I59" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="J59" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">	FechaEntrega DateTime NULL, </v>
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">	IdentificadorReq nVarChar(350) NULL, </v>
       </c>
       <c r="K59" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">	FechaEntrega DateTime NULL, </v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">	IdentificadorReq nVarChar(350) NULL, </v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C60" s="1">
+        <v>0</v>
+      </c>
+      <c r="D60" s="1">
+        <v>0</v>
+      </c>
+      <c r="I60" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="J60" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">	FechaRecepcion DateTime NULL, </v>
+      </c>
+      <c r="K60" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">	FechaRecepcion DateTime NULL, </v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A61" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C61" s="1">
+        <v>0</v>
+      </c>
+      <c r="D61" s="1">
+        <v>0</v>
+      </c>
+      <c r="I61" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="J61" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">	FechaEntrega DateTime NULL)
+GO</v>
+      </c>
+      <c r="K61" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">	FechaEntrega DateTime NULL)
+GO</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A62" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B60" s="1" t="s">
+      <c r="B62" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C60" s="1">
+      <c r="C62" s="1">
         <v>350</v>
       </c>
-      <c r="D60" s="1">
-        <v>0</v>
-      </c>
-      <c r="I60" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="J60" s="1" t="str">
-        <f t="shared" si="1"/>
+      <c r="D62" s="1">
+        <v>0</v>
+      </c>
+      <c r="I62" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="J62" s="1" t="str">
+        <f t="shared" si="4"/>
         <v xml:space="preserve">	ObservacionReq nVarChar(350) NULL, </v>
       </c>
-      <c r="K60" s="1" t="str">
+      <c r="K62" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">	ObservacionReq nVarChar(350) NULL, </v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B63" s="2" t="str">
+        <f>_xlfn.CONCAT("	CONSTRAINT AK_", $C$47, "  UNIQUE (",$A$54,")")</f>
+        <v xml:space="preserve">	CONSTRAINT AK_DatosReqs  UNIQUE (Requerimiento)</v>
+      </c>
+      <c r="I63" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J63" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">	CONSTRAINT AK_DatosReqs  UNIQUE (Requerimiento), </v>
+      </c>
+      <c r="K63" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">	CONSTRAINT AK_DatosReqs  UNIQUE (Requerimiento), </v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I64" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J64" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="K64" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C65" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I65" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>CREATE TABLE DatosPaquete(</v>
+      </c>
+      <c r="J65" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="K65" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>CREATE TABLE DatosPaquete(</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A66" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E66" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F66" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G66" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I66" s="1">
+        <f t="shared" ref="I66:I95" si="5">IF(A66="", IF(C66="", IF(B66="",0,1), _xlfn.CONCAT("CREATE TABLE ",C66,"(")), IF(A66="CAMPO", 0, ""))</f>
+        <v>0</v>
+      </c>
+      <c r="J66" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="K66" s="1" t="str">
+        <f t="shared" ref="K66:K95" si="6">IF(I66=0, "", IF(J66="", I66, J66))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A67" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C67" s="1">
+        <v>0</v>
+      </c>
+      <c r="D67" s="1">
+        <v>1</v>
+      </c>
+      <c r="E67" s="1">
+        <v>1</v>
+      </c>
+      <c r="F67" s="1">
+        <v>1</v>
+      </c>
+      <c r="I67" s="1" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">	ObservacionReq nVarChar(350) NULL, </v>
-      </c>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B61" s="2" t="str">
-        <f>_xlfn.CONCAT("	CONSTRAINT AK_", $C$45, "  UNIQUE (",$A$52,")")</f>
-        <v xml:space="preserve">	CONSTRAINT AK_DatosReqs  UNIQUE (Requerimiento)</v>
-      </c>
-      <c r="I61" s="1">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="J61" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">	CONSTRAINT AK_DatosReqs  UNIQUE (Requerimiento), </v>
-      </c>
-      <c r="K61" s="1" t="str">
+        <v/>
+      </c>
+      <c r="J67" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">	nIdPaquete INT NOT NULL IDENTITY(1,1) PRIMARY KEY, </v>
+      </c>
+      <c r="K67" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">	nIdPaquete INT NOT NULL IDENTITY(1,1) PRIMARY KEY, </v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A68" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C68" s="1">
+        <v>0</v>
+      </c>
+      <c r="D68" s="1">
+        <v>1</v>
+      </c>
+      <c r="G68" s="1" t="str">
+        <f>_xlfn.CONCAT("REFERENCES ", $C$47, "(", $A$49, ")")</f>
+        <v>REFERENCES DatosReqs(nIdRequerimiento)</v>
+      </c>
+      <c r="I68" s="1" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">	CONSTRAINT AK_DatosReqs  UNIQUE (Requerimiento), </v>
-      </c>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="I62" s="1">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="J62" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="K62" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C63" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I63" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>CREATE TABLE DatosPaquete(</v>
-      </c>
-      <c r="J63" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="K63" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>CREATE TABLE DatosPaquete(</v>
-      </c>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A64" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B64" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C64" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D64" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E64" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F64" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G64" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="I64" s="1">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="J64" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="K64" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-    </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A65" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C65" s="1">
-        <v>0</v>
-      </c>
-      <c r="D65" s="1">
-        <v>1</v>
-      </c>
-      <c r="E65" s="1">
-        <v>1</v>
-      </c>
-      <c r="F65" s="1">
-        <v>1</v>
-      </c>
-      <c r="I65" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="J65" s="1" t="str">
-        <f t="shared" ref="J65:J93" si="6">IF(I65="",_xlfn.CONCAT("	", A65," ",B65,IF(C65&gt;0,_xlfn.CONCAT("(",C65,")"),""),IF(D65=1," NOT NULL"," NULL"),IF(F65=1," IDENTITY(1,1)",""),IF(E65=1," PRIMARY KEY",""),IF(G65&lt;&gt;"",_xlfn.CONCAT(" ",G65),""),IF(I66=0,")
-GO",", ")),IF(I65=1,_xlfn.CONCAT(B65,", "), ""))</f>
-        <v xml:space="preserve">	nIdPaquete INT NOT NULL IDENTITY(1,1) PRIMARY KEY, </v>
-      </c>
-      <c r="K65" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">	nIdPaquete INT NOT NULL IDENTITY(1,1) PRIMARY KEY, </v>
-      </c>
-    </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A66" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C66" s="1">
-        <v>0</v>
-      </c>
-      <c r="D66" s="1">
-        <v>1</v>
-      </c>
-      <c r="G66" s="1" t="str">
-        <f>_xlfn.CONCAT("REFERENCES ", $C$45, "(", $A$47, ")")</f>
-        <v>REFERENCES DatosReqs(nIdRequerimiento)</v>
-      </c>
-      <c r="I66" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="J66" s="1" t="str">
+        <v/>
+      </c>
+      <c r="J68" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">	nIdRequerimiento INT NOT NULL REFERENCES DatosReqs(nIdRequerimiento), </v>
+      </c>
+      <c r="K68" s="1" t="str">
         <f t="shared" si="6"/>
         <v xml:space="preserve">	nIdRequerimiento INT NOT NULL REFERENCES DatosReqs(nIdRequerimiento), </v>
       </c>
-      <c r="K66" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">	nIdRequerimiento INT NOT NULL REFERENCES DatosReqs(nIdRequerimiento), </v>
-      </c>
-    </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A67" s="1" t="s">
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A69" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B67" s="1" t="s">
+      <c r="B69" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C67" s="1">
-        <v>0</v>
-      </c>
-      <c r="D67" s="1">
-        <v>1</v>
-      </c>
-      <c r="G67" s="1" t="str">
+      <c r="C69" s="1">
+        <v>0</v>
+      </c>
+      <c r="D69" s="1">
+        <v>1</v>
+      </c>
+      <c r="G69" s="1" t="str">
         <f>_xlfn.CONCAT("REFERENCES ", $C$8, "(", $A$10, ")")</f>
         <v>REFERENCES TablasDetalles(nIdTablaDetalle)</v>
       </c>
-      <c r="I67" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="J67" s="1" t="str">
+      <c r="I69" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="J69" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">	nIdRepositorio INT NOT NULL REFERENCES TablasDetalles(nIdTablaDetalle), </v>
+      </c>
+      <c r="K69" s="1" t="str">
         <f t="shared" si="6"/>
         <v xml:space="preserve">	nIdRepositorio INT NOT NULL REFERENCES TablasDetalles(nIdTablaDetalle), </v>
       </c>
-      <c r="K67" s="1" t="str">
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A70" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C70" s="1">
+        <v>15</v>
+      </c>
+      <c r="D70" s="1">
+        <v>0</v>
+      </c>
+      <c r="I70" s="1" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">	nIdRepositorio INT NOT NULL REFERENCES TablasDetalles(nIdTablaDetalle), </v>
-      </c>
-    </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A68" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B68" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C68" s="1">
-        <v>15</v>
-      </c>
-      <c r="D68" s="1">
-        <v>0</v>
-      </c>
-      <c r="I68" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="J68" s="1" t="str">
+        <v/>
+      </c>
+      <c r="J70" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">	Paquete nChar(15) NULL, </v>
+      </c>
+      <c r="K70" s="1" t="str">
         <f t="shared" si="6"/>
         <v xml:space="preserve">	Paquete nChar(15) NULL, </v>
       </c>
-      <c r="K68" s="1" t="str">
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A71" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C71" s="1">
+        <v>50</v>
+      </c>
+      <c r="D71" s="1">
+        <v>0</v>
+      </c>
+      <c r="I71" s="1" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">	Paquete nChar(15) NULL, </v>
-      </c>
-    </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A69" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B69" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C69" s="1">
-        <v>50</v>
-      </c>
-      <c r="D69" s="1">
-        <v>0</v>
-      </c>
-      <c r="I69" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="J69" s="1" t="str">
+        <v/>
+      </c>
+      <c r="J71" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">	Repositorio nVarChar(50) NULL, </v>
+      </c>
+      <c r="K71" s="1" t="str">
         <f t="shared" si="6"/>
         <v xml:space="preserve">	Repositorio nVarChar(50) NULL, </v>
       </c>
-      <c r="K69" s="1" t="str">
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A72" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C72" s="1">
+        <v>50</v>
+      </c>
+      <c r="D72" s="1">
+        <v>0</v>
+      </c>
+      <c r="I72" s="1" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">	Repositorio nVarChar(50) NULL, </v>
-      </c>
-    </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A70" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B70" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C70" s="1">
-        <v>50</v>
-      </c>
-      <c r="D70" s="1">
-        <v>0</v>
-      </c>
-      <c r="I70" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="J70" s="1" t="str">
+        <v/>
+      </c>
+      <c r="J72" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">	Version nVarChar(50) NULL, </v>
+      </c>
+      <c r="K72" s="1" t="str">
         <f t="shared" si="6"/>
         <v xml:space="preserve">	Version nVarChar(50) NULL, </v>
       </c>
-      <c r="K70" s="1" t="str">
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A73" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C73" s="1">
+        <v>350</v>
+      </c>
+      <c r="D73" s="1">
+        <v>0</v>
+      </c>
+      <c r="I73" s="1" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">	Version nVarChar(50) NULL, </v>
-      </c>
-    </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A71" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C71" s="1">
-        <v>350</v>
-      </c>
-      <c r="D71" s="1">
-        <v>0</v>
-      </c>
-      <c r="I71" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="J71" s="1" t="str">
+        <v/>
+      </c>
+      <c r="J73" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">	Resumen nVarChar(350) NULL, </v>
+      </c>
+      <c r="K73" s="1" t="str">
         <f t="shared" si="6"/>
         <v xml:space="preserve">	Resumen nVarChar(350) NULL, </v>
       </c>
-      <c r="K71" s="1" t="str">
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A74" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C74" s="1">
+        <v>350</v>
+      </c>
+      <c r="D74" s="1">
+        <v>0</v>
+      </c>
+      <c r="I74" s="1" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">	Resumen nVarChar(350) NULL, </v>
-      </c>
-    </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A72" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B72" s="1" t="s">
+        <v/>
+      </c>
+      <c r="J74" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">	IdentificadorPaq nVarChar(350) NULL)
+GO</v>
+      </c>
+      <c r="K74" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">	IdentificadorPaq nVarChar(350) NULL)
+GO</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A75" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B75" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C72" s="1">
+      <c r="C75" s="1">
         <v>350</v>
       </c>
-      <c r="D72" s="1">
-        <v>0</v>
-      </c>
-      <c r="I72" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="J72" s="1" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve">	IdentificadorPaq nVarChar(350) NULL, </v>
-      </c>
-      <c r="K72" s="1" t="str">
+      <c r="D75" s="1">
+        <v>0</v>
+      </c>
+      <c r="I75" s="1" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">	IdentificadorPaq nVarChar(350) NULL, </v>
-      </c>
-    </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A73" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B73" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C73" s="1">
-        <v>350</v>
-      </c>
-      <c r="D73" s="1">
-        <v>0</v>
-      </c>
-      <c r="I73" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="J73" s="1" t="str">
+        <v/>
+      </c>
+      <c r="J75" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">	ObservacionPaq nVarChar(350) NULL, </v>
+      </c>
+      <c r="K75" s="1" t="str">
         <f t="shared" si="6"/>
         <v xml:space="preserve">	ObservacionPaq nVarChar(350) NULL, </v>
       </c>
-      <c r="K73" s="1" t="str">
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B76" s="2" t="str">
+        <f>_xlfn.CONCAT("	CONSTRAINT AK_", $C$65, "  UNIQUE (",$A$70,")")</f>
+        <v xml:space="preserve">	CONSTRAINT AK_DatosPaquete  UNIQUE (Paquete)</v>
+      </c>
+      <c r="I76" s="1">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">	ObservacionPaq nVarChar(350) NULL, </v>
-      </c>
-    </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B74" s="2" t="str">
-        <f>_xlfn.CONCAT("	CONSTRAINT AK_", $C$63, "  UNIQUE (",$A$68,")")</f>
-        <v xml:space="preserve">	CONSTRAINT AK_DatosPaquete  UNIQUE (Paquete)</v>
-      </c>
-      <c r="I74" s="1">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="J74" s="1" t="str">
+        <v>1</v>
+      </c>
+      <c r="J76" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">	CONSTRAINT AK_DatosPaquete  UNIQUE (Paquete), </v>
+      </c>
+      <c r="K76" s="1" t="str">
         <f t="shared" si="6"/>
         <v xml:space="preserve">	CONSTRAINT AK_DatosPaquete  UNIQUE (Paquete), </v>
       </c>
-      <c r="K74" s="1" t="str">
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I77" s="1">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">	CONSTRAINT AK_DatosPaquete  UNIQUE (Paquete), </v>
-      </c>
-    </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="I75" s="1">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="J75" s="1" t="str">
+        <v>0</v>
+      </c>
+      <c r="J77" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="K77" s="1" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="K75" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-    </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C76" s="1" t="s">
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C78" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="I76" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>CREATE TABLE DatosRDL(</v>
-      </c>
-      <c r="J76" s="1" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="K76" s="1" t="str">
+      <c r="I78" s="1" t="str">
         <f t="shared" si="5"/>
         <v>CREATE TABLE DatosRDL(</v>
       </c>
-    </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A77" s="3" t="s">
+      <c r="J78" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="K78" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>CREATE TABLE DatosRDL(</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A79" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B77" s="3" t="s">
+      <c r="B79" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C77" s="3" t="s">
+      <c r="C79" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D77" s="3" t="s">
+      <c r="D79" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E77" s="3" t="s">
+      <c r="E79" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F77" s="3" t="s">
+      <c r="F79" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G77" s="3" t="s">
+      <c r="G79" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="I77" s="1">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="J77" s="1" t="str">
+      <c r="I79" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J79" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="K79" s="1" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="K77" s="1" t="str">
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A80" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C80" s="1">
+        <v>0</v>
+      </c>
+      <c r="D80" s="1">
+        <v>1</v>
+      </c>
+      <c r="E80" s="1">
+        <v>1</v>
+      </c>
+      <c r="F80" s="1">
+        <v>1</v>
+      </c>
+      <c r="I80" s="1" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-    </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A78" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B78" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C78" s="1">
-        <v>0</v>
-      </c>
-      <c r="D78" s="1">
-        <v>1</v>
-      </c>
-      <c r="E78" s="1">
-        <v>1</v>
-      </c>
-      <c r="F78" s="1">
-        <v>1</v>
-      </c>
-      <c r="I78" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="J78" s="1" t="str">
+      <c r="J80" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">	nIdRDL INT NOT NULL IDENTITY(1,1) PRIMARY KEY, </v>
+      </c>
+      <c r="K80" s="1" t="str">
         <f t="shared" si="6"/>
         <v xml:space="preserve">	nIdRDL INT NOT NULL IDENTITY(1,1) PRIMARY KEY, </v>
       </c>
-      <c r="K78" s="1" t="str">
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A81" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C81" s="1">
+        <v>0</v>
+      </c>
+      <c r="D81" s="1">
+        <v>1</v>
+      </c>
+      <c r="G81" s="1" t="str">
+        <f>_xlfn.CONCAT("REFERENCES ", $C$65, "(", $A$67, ")")</f>
+        <v>REFERENCES DatosPaquete(nIdPaquete)</v>
+      </c>
+      <c r="I81" s="1" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">	nIdRDL INT NOT NULL IDENTITY(1,1) PRIMARY KEY, </v>
-      </c>
-    </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A79" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B79" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C79" s="1">
-        <v>0</v>
-      </c>
-      <c r="D79" s="1">
-        <v>1</v>
-      </c>
-      <c r="G79" s="1" t="str">
-        <f>_xlfn.CONCAT("REFERENCES ", $C$63, "(", $A$65, ")")</f>
-        <v>REFERENCES DatosPaquete(nIdPaquete)</v>
-      </c>
-      <c r="I79" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="J79" s="1" t="str">
+        <v/>
+      </c>
+      <c r="J81" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">	nIdPaquete INT NOT NULL REFERENCES DatosPaquete(nIdPaquete), </v>
+      </c>
+      <c r="K81" s="1" t="str">
         <f t="shared" si="6"/>
         <v xml:space="preserve">	nIdPaquete INT NOT NULL REFERENCES DatosPaquete(nIdPaquete), </v>
       </c>
-      <c r="K79" s="1" t="str">
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A82" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C82" s="1">
+        <v>0</v>
+      </c>
+      <c r="D82" s="1">
+        <v>1</v>
+      </c>
+      <c r="I82" s="1" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">	nIdPaquete INT NOT NULL REFERENCES DatosPaquete(nIdPaquete), </v>
-      </c>
-    </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A80" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B80" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C80" s="1">
-        <v>0</v>
-      </c>
-      <c r="D80" s="1">
-        <v>1</v>
-      </c>
-      <c r="I80" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="J80" s="1" t="str">
+        <v/>
+      </c>
+      <c r="J82" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">	RDL INT NOT NULL, </v>
+      </c>
+      <c r="K82" s="1" t="str">
         <f t="shared" si="6"/>
         <v xml:space="preserve">	RDL INT NOT NULL, </v>
       </c>
-      <c r="K80" s="1" t="str">
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A83" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C83" s="1">
+        <v>12</v>
+      </c>
+      <c r="I83" s="1" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">	RDL INT NOT NULL, </v>
-      </c>
-    </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A81" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B81" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C81" s="1">
-        <v>12</v>
-      </c>
-      <c r="I81" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="J81" s="1" t="str">
+        <v/>
+      </c>
+      <c r="J83" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">	Paquete nVarChar(12) NULL, </v>
+      </c>
+      <c r="K83" s="1" t="str">
         <f t="shared" si="6"/>
         <v xml:space="preserve">	Paquete nVarChar(12) NULL, </v>
       </c>
-      <c r="K81" s="1" t="str">
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A84" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C84" s="1">
+        <v>0</v>
+      </c>
+      <c r="I84" s="1" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">	Paquete nVarChar(12) NULL, </v>
-      </c>
-    </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A82" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B82" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C82" s="1">
-        <v>0</v>
-      </c>
-      <c r="I82" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="J82" s="1" t="str">
+        <v/>
+      </c>
+      <c r="J84" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">	FechaInicio DateTime NULL, </v>
+      </c>
+      <c r="K84" s="1" t="str">
         <f t="shared" si="6"/>
         <v xml:space="preserve">	FechaInicio DateTime NULL, </v>
       </c>
-      <c r="K82" s="1" t="str">
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A85" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C85" s="1">
+        <v>0</v>
+      </c>
+      <c r="I85" s="1" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">	FechaInicio DateTime NULL, </v>
-      </c>
-    </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A83" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B83" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C83" s="1">
-        <v>0</v>
-      </c>
-      <c r="I83" s="1" t="str">
-        <f t="shared" ref="I83:I93" si="7">IF(A83="", IF(C83="", IF(B83="",0,1), _xlfn.CONCAT("CREATE TABLE ",C83,"(")), IF(A83="CAMPO", 0, ""))</f>
-        <v/>
-      </c>
-      <c r="J83" s="1" t="str">
+        <v/>
+      </c>
+      <c r="J85" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">	FechaFin DateTime NULL)
+GO</v>
+      </c>
+      <c r="K85" s="1" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">	FechaFin DateTime NULL, </v>
-      </c>
-      <c r="K83" s="1" t="str">
-        <f t="shared" ref="K83:K93" si="8">IF(I83=0, "", IF(J83="", I83, J83))</f>
-        <v xml:space="preserve">	FechaFin DateTime NULL, </v>
-      </c>
-    </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A84" s="1" t="s">
+        <v xml:space="preserve">	FechaFin DateTime NULL)
+GO</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A86" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B84" s="1" t="s">
+      <c r="B86" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C84" s="1">
-        <v>0</v>
-      </c>
-      <c r="I84" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="J84" s="1" t="str">
+      <c r="C86" s="1">
+        <v>0</v>
+      </c>
+      <c r="I86" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="J86" s="1" t="str">
+        <f t="shared" ref="J86:J95" si="7">IF(I86="",_xlfn.CONCAT("	", A86," ",B86,IF(C86&gt;0,_xlfn.CONCAT("(",C86,")"),""),IF(D86=1," NOT NULL"," NULL"),IF(F86=1," IDENTITY(1,1)",""),IF(E86=1," PRIMARY KEY",""),IF(G86&lt;&gt;"",_xlfn.CONCAT(" ",G86),""),IF(I89=0,")
+GO",", ")),IF(I86=1,_xlfn.CONCAT(B86,", "), ""))</f>
+        <v xml:space="preserve">	Id_Estado Int NULL, </v>
+      </c>
+      <c r="K86" s="1" t="str">
         <f t="shared" si="6"/>
         <v xml:space="preserve">	Id_Estado Int NULL, </v>
       </c>
-      <c r="K84" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v xml:space="preserve">	Id_Estado Int NULL, </v>
-      </c>
-    </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A85" s="1" t="s">
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A87" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B85" s="1" t="s">
+      <c r="B87" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C85" s="1">
-        <v>0</v>
-      </c>
-      <c r="I85" s="1" t="str">
+      <c r="C87" s="1">
+        <v>0</v>
+      </c>
+      <c r="I87" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="J87" s="1" t="str">
         <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="J85" s="1" t="str">
+        <v xml:space="preserve">	Id_Responsable Int NULL)
+GO</v>
+      </c>
+      <c r="K87" s="1" t="str">
         <f t="shared" si="6"/>
         <v xml:space="preserve">	Id_Responsable Int NULL)
 GO</v>
       </c>
-      <c r="K85" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v xml:space="preserve">	Id_Responsable Int NULL)
-GO</v>
-      </c>
-    </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="I86" s="1">
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I88" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J88" s="1" t="str">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="J86" s="1" t="str">
+        <v/>
+      </c>
+      <c r="K88" s="1" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="K86" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-    </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C87" s="1" t="s">
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C89" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="I87" s="1" t="str">
+      <c r="I89" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>CREATE TABLE Observacioines(</v>
+      </c>
+      <c r="J89" s="1" t="str">
         <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="K89" s="1" t="str">
+        <f t="shared" si="6"/>
         <v>CREATE TABLE Observacioines(</v>
       </c>
-      <c r="J87" s="1" t="str">
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A90" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B90" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C90" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D90" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E90" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F90" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G90" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I90" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J90" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="K90" s="1" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="K87" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v>CREATE TABLE Observacioines(</v>
-      </c>
-    </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A88" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B88" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C88" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D88" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E88" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F88" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G88" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="I88" s="1">
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A91" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C91" s="1">
+        <v>0</v>
+      </c>
+      <c r="D91" s="1">
+        <v>1</v>
+      </c>
+      <c r="E91" s="1">
+        <v>1</v>
+      </c>
+      <c r="F91" s="1">
+        <v>1</v>
+      </c>
+      <c r="I91" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="J91" s="1" t="str">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="J88" s="1" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="K88" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-    </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A89" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B89" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C89" s="1">
-        <v>0</v>
-      </c>
-      <c r="D89" s="1">
-        <v>1</v>
-      </c>
-      <c r="E89" s="1">
-        <v>1</v>
-      </c>
-      <c r="F89" s="1">
-        <v>1</v>
-      </c>
-      <c r="I89" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="J89" s="1" t="str">
+        <v xml:space="preserve">	nIdObservaciones INT NOT NULL IDENTITY(1,1) PRIMARY KEY, </v>
+      </c>
+      <c r="K91" s="1" t="str">
         <f t="shared" si="6"/>
         <v xml:space="preserve">	nIdObservaciones INT NOT NULL IDENTITY(1,1) PRIMARY KEY, </v>
       </c>
-      <c r="K89" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v xml:space="preserve">	nIdObservaciones INT NOT NULL IDENTITY(1,1) PRIMARY KEY, </v>
-      </c>
-    </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A90" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B90" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C90" s="1">
-        <v>0</v>
-      </c>
-      <c r="D90" s="1">
-        <v>0</v>
-      </c>
-      <c r="G90" s="1" t="str">
-        <f>_xlfn.CONCAT("REFERENCES ", $C$45, "(", $A$47, ")")</f>
-        <v>REFERENCES DatosReqs(nIdRequerimiento)</v>
-      </c>
-      <c r="I90" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="J90" s="1" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve">	nIdRequerimiento INT NULL REFERENCES DatosReqs(nIdRequerimiento), </v>
-      </c>
-      <c r="K90" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v xml:space="preserve">	nIdRequerimiento INT NULL REFERENCES DatosReqs(nIdRequerimiento), </v>
-      </c>
-    </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A91" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B91" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C91" s="1">
-        <v>0</v>
-      </c>
-      <c r="D91" s="1">
-        <v>0</v>
-      </c>
-      <c r="G91" s="1" t="str">
-        <f>_xlfn.CONCAT("REFERENCES ", $C$63, "(", $A$65, ")")</f>
-        <v>REFERENCES DatosPaquete(nIdPaquete)</v>
-      </c>
-      <c r="I91" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="J91" s="1" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve">	nIdPaquete INT NULL REFERENCES DatosPaquete(nIdPaquete), </v>
-      </c>
-      <c r="K91" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v xml:space="preserve">	nIdPaquete INT NULL REFERENCES DatosPaquete(nIdPaquete), </v>
-      </c>
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C92" s="1">
+        <v>0</v>
+      </c>
+      <c r="D92" s="1">
+        <v>0</v>
+      </c>
+      <c r="G92" s="1" t="str">
+        <f>_xlfn.CONCAT("REFERENCES ", $C$47, "(", $A$49, ")")</f>
+        <v>REFERENCES DatosReqs(nIdRequerimiento)</v>
+      </c>
+      <c r="I92" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="J92" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">	nIdRequerimiento INT NULL REFERENCES DatosReqs(nIdRequerimiento))
+GO</v>
+      </c>
+      <c r="K92" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">	nIdRequerimiento INT NULL REFERENCES DatosReqs(nIdRequerimiento))
+GO</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A93" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C93" s="1">
+        <v>0</v>
+      </c>
+      <c r="D93" s="1">
+        <v>0</v>
+      </c>
+      <c r="G93" s="1" t="str">
+        <f>_xlfn.CONCAT("REFERENCES ", $C$65, "(", $A$67, ")")</f>
+        <v>REFERENCES DatosPaquete(nIdPaquete)</v>
+      </c>
+      <c r="I93" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="J93" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">	nIdPaquete INT NULL REFERENCES DatosPaquete(nIdPaquete))
+GO</v>
+      </c>
+      <c r="K93" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">	nIdPaquete INT NULL REFERENCES DatosPaquete(nIdPaquete))
+GO</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A94" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B92" s="1" t="s">
+      <c r="B94" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C92" s="1">
+      <c r="C94" s="1">
         <v>350</v>
       </c>
-      <c r="D92" s="1">
-        <v>0</v>
-      </c>
-      <c r="I92" s="1" t="str">
+      <c r="D94" s="1">
+        <v>0</v>
+      </c>
+      <c r="I94" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="J94" s="1" t="str">
         <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="J92" s="1" t="str">
+        <v xml:space="preserve">	Observacion nVarChar(350) NULL)
+GO</v>
+      </c>
+      <c r="K94" s="1" t="str">
         <f t="shared" si="6"/>
         <v xml:space="preserve">	Observacion nVarChar(350) NULL)
 GO</v>
       </c>
-      <c r="K92" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v xml:space="preserve">	Observacion nVarChar(350) NULL)
-GO</v>
-      </c>
-    </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="I93" s="1">
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I95" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J95" s="1" t="str">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="J93" s="1" t="str">
+        <v/>
+      </c>
+      <c r="K95" s="1" t="str">
         <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="K93" s="1" t="str">
-        <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
@@ -3336,10 +3440,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E7C2D72-1FAE-4DEA-8254-172C45BBECDF}">
-  <dimension ref="A1:W69"/>
+  <dimension ref="A1:Y79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="U5" sqref="U5"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="Y2" sqref="Y2:Y6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -3351,19 +3455,19 @@
     <col min="5" max="5" width="5.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="35.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.7109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="5.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="4.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="5.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="11.42578125" style="1"/>
+    <col min="8" max="10" width="11.7109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="5.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="4.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="5.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>17</v>
       </c>
@@ -3382,44 +3486,50 @@
       <c r="G1" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>26</v>
       </c>
@@ -3443,56 +3553,59 @@
         <f>_xlfn.CONCAT("INSERT INTO ",Hoja2!$C$8, " (", $C$1, ", ", $D$1, ", ", $E$1, ", ", $F$1, ", ", $G$1, ", Estado) VALUES(", C2, ", '", D2, "', ", E2, ", '", F2, "', '", G2, "', 1)")</f>
         <v>INSERT INTO TablasDetalles (nIdTabla, Acronimo, Orden, TablaDetalle, Observaciones, Estado) VALUES(1, 'RMA', 0, 'RMA', '', 1)</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" s="1">
+        <v>8</v>
+      </c>
+      <c r="K2" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="N2" s="1">
+      <c r="P2" s="1">
         <v>3</v>
       </c>
-      <c r="O2" s="1">
-        <v>0</v>
-      </c>
-      <c r="P2" s="1">
-        <v>1</v>
-      </c>
-      <c r="Q2" s="1" t="str">
-        <f>_xlfn.CONCAT("INSERT INTO ",Hoja2!$C$19, " (",$I$1, ", ", $J$1, ", ", $K$1, ", ", $L$1, ", ", $M$1, ", ", $N$1, ", ", $O$1, ", ", $P$1, ") VALUES('", I2, "', '", J2, "', ", K2, ", '", L2, "', '", M2, "', ", N2, ", ", O2, ", ", P2, ")")</f>
-        <v>INSERT INTO Empleados (sNombre, sApellido1, sApellido2, sUsuario, sContra, Orden, Root, Estado) VALUES('ISAAC', 'DIAS', VARGAS, 'idias', 'oEFPCa1Z1k+qV2t65a98yA==', 3, 0, 1)</v>
+      <c r="Q2" s="1">
+        <v>0</v>
       </c>
       <c r="R2" s="1">
         <v>1</v>
       </c>
-      <c r="S2" s="1">
-        <v>8</v>
-      </c>
-      <c r="T2" s="1" t="str">
-        <f>_xlfn.CONCAT("INSERT INTO ", Hoja2!$C$33, " (", $R$1, ", ", $S$1, ") VALUES(", R2, ", ", S2, ")")</f>
-        <v>INSERT INTO EmpleadoArea (nIdEmpleado, nIdArea) VALUES(1, 8)</v>
+      <c r="S2" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO ",Hoja2!$C$19, " (", $I$1, ", ", $J$1, ", ",$K$1, ", ", $L$1, ", ", $M$1, ", ", $N$1, ", ", $O$1, ", ", $P$1, ", ", $Q$1, ", ", $R$1, ") VALUES(", I2, ", null, '", K2, "', '", L2, "', ", M2, ", '", N2, "', '", O2, "', ", P2, ", ", Q2, ", ", R2, ")")</f>
+        <v>INSERT INTO Empleados (nIdArea, nIdAplicativo, sNombre, sApellido1, sApellido2, sUsuario, sContra, Orden, Root, Estado) VALUES(8, null, 'ISAAC', 'DIAS', VARGAS, 'idias', 'oEFPCa1Z1k+qV2t65a98yA==', 3, 0, 1)</v>
+      </c>
+      <c r="T2" s="1">
+        <v>1</v>
       </c>
       <c r="U2" s="1">
         <v>8</v>
       </c>
-      <c r="V2" s="1">
+      <c r="V2" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO ", Hoja2!$C$35, " (", $T$1, ", ", $U$1, ") VALUES(", T2, ", ", U2, ")")</f>
+        <v>INSERT INTO EmpleadoArea (nIdEmpleado, nIdArea) VALUES(1, 8)</v>
+      </c>
+      <c r="W2" s="1">
+        <v>8</v>
+      </c>
+      <c r="X2" s="1">
         <v>59</v>
       </c>
-      <c r="W2" s="1" t="str">
-        <f>_xlfn.CONCAT("INSERT INTO ", Hoja2!$C$39, " (", $U$1, ", ", $V$1, ") VALUES(", U2, ", ", V2, ")")</f>
+      <c r="Y2" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO ", Hoja2!$C$41, " (", $W$1, ", ", $X$1, ") VALUES(", W2, ", ", X2, ")")</f>
         <v>INSERT INTO AreaAplicativo (nIdArea, nIdAplicativo) VALUES(8, 59)</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>35</v>
       </c>
@@ -3516,56 +3629,59 @@
         <f>_xlfn.CONCAT("INSERT INTO ",Hoja2!$C$8, " (", $C$1, ", ", $D$1, ", ", $E$1, ", ", $F$1, ", ", $G$1, ", Estado) VALUES(", C3, ", '", D3, "', ", E3, ", '", F3, "', '", G3, "', 1)")</f>
         <v>INSERT INTO TablasDetalles (nIdTabla, Acronimo, Orden, TablaDetalle, Observaciones, Estado) VALUES(1, 'POL', 0, 'POL', '', 1)</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="I3" s="1">
+        <v>8</v>
+      </c>
+      <c r="K3" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="L3" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="M3" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="N3" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="O3" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="N3" s="1">
+      <c r="P3" s="1">
         <v>4</v>
       </c>
-      <c r="O3" s="1">
-        <v>0</v>
-      </c>
-      <c r="P3" s="1">
-        <v>1</v>
-      </c>
-      <c r="Q3" s="1" t="str">
-        <f>_xlfn.CONCAT("INSERT INTO ",Hoja2!$C$19, " (",$I$1, ", ", $J$1, ", ", $K$1, ", ", $L$1, ", ", $M$1, ", ", $N$1, ", ", $O$1, ", ", $P$1, ") VALUES('", I3, "', '", J3, "', ", K3, ", '", L3, "', '", M3, "', ", N3, ", ", O3, ", ", P3, ")")</f>
-        <v>INSERT INTO Empleados (sNombre, sApellido1, sApellido2, sUsuario, sContra, Orden, Root, Estado) VALUES('JOSE ANTONIO', 'MENDOSA', SALASAR, 'jmendosa', 'oEFPCa1Z1k+qV2t65a98yA==', 4, 0, 1)</v>
+      <c r="Q3" s="1">
+        <v>0</v>
       </c>
       <c r="R3" s="1">
+        <v>1</v>
+      </c>
+      <c r="S3" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO ",Hoja2!$C$19, " (", $I$1, ", ", $J$1, ", ",$K$1, ", ", $L$1, ", ", $M$1, ", ", $N$1, ", ", $O$1, ", ", $P$1, ", ", $Q$1, ", ", $R$1, ") VALUES(", I3, ", null, '", K3, "', '", L3, "', ", M3, ", '", N3, "', '", O3, "', ", P3, ", ", Q3, ", ", R3, ")")</f>
+        <v>INSERT INTO Empleados (nIdArea, nIdAplicativo, sNombre, sApellido1, sApellido2, sUsuario, sContra, Orden, Root, Estado) VALUES(8, null, 'JOSE ANTONIO', 'MENDOSA', SALASAR, 'jmendosa', 'oEFPCa1Z1k+qV2t65a98yA==', 4, 0, 1)</v>
+      </c>
+      <c r="T3" s="1">
         <v>2</v>
-      </c>
-      <c r="S3" s="1">
-        <v>8</v>
-      </c>
-      <c r="T3" s="1" t="str">
-        <f>_xlfn.CONCAT("INSERT INTO ", Hoja2!$C$33, " (", $R$1, ", ", $S$1, ") VALUES(", R3, ", ", S3, ")")</f>
-        <v>INSERT INTO EmpleadoArea (nIdEmpleado, nIdArea) VALUES(2, 8)</v>
       </c>
       <c r="U3" s="1">
         <v>8</v>
       </c>
-      <c r="V3" s="1">
+      <c r="V3" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO ", Hoja2!$C$35, " (", $T$1, ", ", $U$1, ") VALUES(", T3, ", ", U3, ")")</f>
+        <v>INSERT INTO EmpleadoArea (nIdEmpleado, nIdArea) VALUES(2, 8)</v>
+      </c>
+      <c r="W3" s="1">
+        <v>8</v>
+      </c>
+      <c r="X3" s="1">
         <v>60</v>
       </c>
-      <c r="W3" s="1" t="str">
-        <f>_xlfn.CONCAT("INSERT INTO ", Hoja2!$C$39, " (", $U$1, ", ", $V$1, ") VALUES(", U3, ", ", V3, ")")</f>
+      <c r="Y3" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO ", Hoja2!$C$41, " (", $W$1, ", ", $X$1, ") VALUES(", W3, ", ", X3, ")")</f>
         <v>INSERT INTO AreaAplicativo (nIdArea, nIdAplicativo) VALUES(8, 60)</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>167</v>
       </c>
@@ -3589,56 +3705,59 @@
         <f>_xlfn.CONCAT("INSERT INTO ",Hoja2!$C$8, " (", $C$1, ", ", $D$1, ", ", $E$1, ", ", $F$1, ", ", $G$1, ", Estado) VALUES(", C4, ", '", D4, "', ", E4, ", '", F4, "', '", G4, "', 1)")</f>
         <v>INSERT INTO TablasDetalles (nIdTabla, Acronimo, Orden, TablaDetalle, Observaciones, Estado) VALUES(2, 'Reg', 0, 'Registrado', '', 1)</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="I4" s="1">
+        <v>8</v>
+      </c>
+      <c r="K4" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="L4" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="M4" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="N4" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="M4" s="1" t="s">
+      <c r="O4" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="N4" s="1">
-        <v>1</v>
-      </c>
-      <c r="O4" s="1">
-        <v>1</v>
-      </c>
       <c r="P4" s="1">
         <v>1</v>
       </c>
-      <c r="Q4" s="1" t="str">
-        <f>_xlfn.CONCAT("INSERT INTO ",Hoja2!$C$19, " (",$I$1, ", ", $J$1, ", ", $K$1, ", ", $L$1, ", ", $M$1, ", ", $N$1, ", ", $O$1, ", ", $P$1, ") VALUES('", I4, "', '", J4, "', ", K4, ", '", L4, "', '", M4, "', ", N4, ", ", O4, ", ", P4, ")")</f>
-        <v>INSERT INTO Empleados (sNombre, sApellido1, sApellido2, sUsuario, sContra, Orden, Root, Estado) VALUES('ARTURO EFRAIN', 'MINGUES', ALCANTARA, 'amingues', 'oEFPCa1Z1k+qV2t65a98yA==', 1, 1, 1)</v>
+      <c r="Q4" s="1">
+        <v>1</v>
       </c>
       <c r="R4" s="1">
+        <v>1</v>
+      </c>
+      <c r="S4" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO ",Hoja2!$C$19, " (", $I$1, ", ", $J$1, ", ",$K$1, ", ", $L$1, ", ", $M$1, ", ", $N$1, ", ", $O$1, ", ", $P$1, ", ", $Q$1, ", ", $R$1, ") VALUES(", I4, ", null, '", K4, "', '", L4, "', ", M4, ", '", N4, "', '", O4, "', ", P4, ", ", Q4, ", ", R4, ")")</f>
+        <v>INSERT INTO Empleados (nIdArea, nIdAplicativo, sNombre, sApellido1, sApellido2, sUsuario, sContra, Orden, Root, Estado) VALUES(8, null, 'ARTURO EFRAIN', 'MINGUES', ALCANTARA, 'amingues', 'oEFPCa1Z1k+qV2t65a98yA==', 1, 1, 1)</v>
+      </c>
+      <c r="T4" s="1">
         <v>3</v>
-      </c>
-      <c r="S4" s="1">
-        <v>8</v>
-      </c>
-      <c r="T4" s="1" t="str">
-        <f>_xlfn.CONCAT("INSERT INTO ", Hoja2!$C$33, " (", $R$1, ", ", $S$1, ") VALUES(", R4, ", ", S4, ")")</f>
-        <v>INSERT INTO EmpleadoArea (nIdEmpleado, nIdArea) VALUES(3, 8)</v>
       </c>
       <c r="U4" s="1">
         <v>8</v>
       </c>
-      <c r="V4" s="1">
+      <c r="V4" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO ", Hoja2!$C$35, " (", $T$1, ", ", $U$1, ") VALUES(", T4, ", ", U4, ")")</f>
+        <v>INSERT INTO EmpleadoArea (nIdEmpleado, nIdArea) VALUES(3, 8)</v>
+      </c>
+      <c r="W4" s="1">
+        <v>8</v>
+      </c>
+      <c r="X4" s="1">
         <v>61</v>
       </c>
-      <c r="W4" s="1" t="str">
-        <f>_xlfn.CONCAT("INSERT INTO ", Hoja2!$C$39, " (", $U$1, ", ", $V$1, ") VALUES(", U4, ", ", V4, ")")</f>
+      <c r="Y4" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO ", Hoja2!$C$41, " (", $W$1, ", ", $X$1, ") VALUES(", W4, ", ", X4, ")")</f>
         <v>INSERT INTO AreaAplicativo (nIdArea, nIdAplicativo) VALUES(8, 61)</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>59</v>
       </c>
@@ -3662,56 +3781,59 @@
         <f>_xlfn.CONCAT("INSERT INTO ",Hoja2!$C$8, " (", $C$1, ", ", $D$1, ", ", $E$1, ", ", $F$1, ", ", $G$1, ", Estado) VALUES(", C5, ", '", D5, "', ", E5, ", '", F5, "', '", G5, "', 1)")</f>
         <v>INSERT INTO TablasDetalles (nIdTabla, Acronimo, Orden, TablaDetalle, Observaciones, Estado) VALUES(2, 'Cur', 0, 'Curso', '', 1)</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="I5" s="1">
+        <v>8</v>
+      </c>
+      <c r="K5" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="L5" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="K5" s="1" t="s">
+      <c r="M5" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="L5" s="1" t="s">
+      <c r="N5" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="M5" s="1" t="s">
+      <c r="O5" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="N5" s="1">
+      <c r="P5" s="1">
         <v>2</v>
       </c>
-      <c r="O5" s="1">
-        <v>1</v>
-      </c>
-      <c r="P5" s="1">
-        <v>1</v>
-      </c>
-      <c r="Q5" s="1" t="str">
-        <f>_xlfn.CONCAT("INSERT INTO ",Hoja2!$C$19, " (",$I$1, ", ", $J$1, ", ", $K$1, ", ", $L$1, ", ", $M$1, ", ", $N$1, ", ", $O$1, ", ", $P$1, ") VALUES('", I5, "', '", J5, "', ", K5, ", '", L5, "', '", M5, "', ", N5, ", ", O5, ", ", P5, ")")</f>
-        <v>INSERT INTO Empleados (sNombre, sApellido1, sApellido2, sUsuario, sContra, Orden, Root, Estado) VALUES('MANUEL FRANCISCO ', 'MUÑOS', CALVO, 'mmuños', 'oEFPCa1Z1k+qV2t65a98yA==', 2, 1, 1)</v>
+      <c r="Q5" s="1">
+        <v>1</v>
       </c>
       <c r="R5" s="1">
+        <v>1</v>
+      </c>
+      <c r="S5" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO ",Hoja2!$C$19, " (", $I$1, ", ", $J$1, ", ",$K$1, ", ", $L$1, ", ", $M$1, ", ", $N$1, ", ", $O$1, ", ", $P$1, ", ", $Q$1, ", ", $R$1, ") VALUES(", I5, ", null, '", K5, "', '", L5, "', ", M5, ", '", N5, "', '", O5, "', ", P5, ", ", Q5, ", ", R5, ")")</f>
+        <v>INSERT INTO Empleados (nIdArea, nIdAplicativo, sNombre, sApellido1, sApellido2, sUsuario, sContra, Orden, Root, Estado) VALUES(8, null, 'MANUEL FRANCISCO ', 'MUÑOS', CALVO, 'mmuños', 'oEFPCa1Z1k+qV2t65a98yA==', 2, 1, 1)</v>
+      </c>
+      <c r="T5" s="1">
         <v>4</v>
-      </c>
-      <c r="S5" s="1">
-        <v>8</v>
-      </c>
-      <c r="T5" s="1" t="str">
-        <f>_xlfn.CONCAT("INSERT INTO ", Hoja2!$C$33, " (", $R$1, ", ", $S$1, ") VALUES(", R5, ", ", S5, ")")</f>
-        <v>INSERT INTO EmpleadoArea (nIdEmpleado, nIdArea) VALUES(4, 8)</v>
       </c>
       <c r="U5" s="1">
         <v>8</v>
       </c>
-      <c r="V5" s="1">
+      <c r="V5" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO ", Hoja2!$C$35, " (", $T$1, ", ", $U$1, ") VALUES(", T5, ", ", U5, ")")</f>
+        <v>INSERT INTO EmpleadoArea (nIdEmpleado, nIdArea) VALUES(4, 8)</v>
+      </c>
+      <c r="W5" s="1">
+        <v>8</v>
+      </c>
+      <c r="X5" s="1">
         <v>62</v>
       </c>
-      <c r="W5" s="1" t="str">
-        <f>_xlfn.CONCAT("INSERT INTO ", Hoja2!$C$39, " (", $U$1, ", ", $V$1, ") VALUES(", U5, ", ", V5, ")")</f>
+      <c r="Y5" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO ", Hoja2!$C$41, " (", $W$1, ", ", $X$1, ") VALUES(", W5, ", ", X5, ")")</f>
         <v>INSERT INTO AreaAplicativo (nIdArea, nIdAplicativo) VALUES(8, 62)</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>58</v>
       </c>
@@ -3735,56 +3857,59 @@
         <f>_xlfn.CONCAT("INSERT INTO ",Hoja2!$C$8, " (", $C$1, ", ", $D$1, ", ", $E$1, ", ", $F$1, ", ", $G$1, ", Estado) VALUES(", C6, ", '", D6, "', ", E6, ", '", F6, "', '", G6, "', 1)")</f>
         <v>INSERT INTO TablasDetalles (nIdTabla, Acronimo, Orden, TablaDetalle, Observaciones, Estado) VALUES(2, 'Paq', 0, 'Paquete', '', 1)</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="I6" s="1">
+        <v>8</v>
+      </c>
+      <c r="K6" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="L6" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="K6" s="1" t="s">
+      <c r="M6" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="L6" s="1" t="s">
+      <c r="N6" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="M6" s="1" t="s">
+      <c r="O6" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="N6" s="1">
+      <c r="P6" s="1">
         <v>6</v>
       </c>
-      <c r="O6" s="1">
-        <v>1</v>
-      </c>
-      <c r="P6" s="1">
-        <v>1</v>
-      </c>
-      <c r="Q6" s="1" t="str">
-        <f>_xlfn.CONCAT("INSERT INTO ",Hoja2!$C$19, " (",$I$1, ", ", $J$1, ", ", $K$1, ", ", $L$1, ", ", $M$1, ", ", $N$1, ", ", $O$1, ", ", $P$1, ") VALUES('", I6, "', '", J6, "', ", K6, ", '", L6, "', '", M6, "', ", N6, ", ", O6, ", ", P6, ")")</f>
-        <v>INSERT INTO Empleados (sNombre, sApellido1, sApellido2, sUsuario, sContra, Orden, Root, Estado) VALUES('ANGEL', 'RAMIREZ', MANCERA, 'aramirez', 'oEFPCa1Z1k+qV2t65a98yA==', 6, 1, 1)</v>
+      <c r="Q6" s="1">
+        <v>1</v>
       </c>
       <c r="R6" s="1">
+        <v>1</v>
+      </c>
+      <c r="S6" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO ",Hoja2!$C$19, " (", $I$1, ", ", $J$1, ", ",$K$1, ", ", $L$1, ", ", $M$1, ", ", $N$1, ", ", $O$1, ", ", $P$1, ", ", $Q$1, ", ", $R$1, ") VALUES(", I6, ", null, '", K6, "', '", L6, "', ", M6, ", '", N6, "', '", O6, "', ", P6, ", ", Q6, ", ", R6, ")")</f>
+        <v>INSERT INTO Empleados (nIdArea, nIdAplicativo, sNombre, sApellido1, sApellido2, sUsuario, sContra, Orden, Root, Estado) VALUES(8, null, 'ANGEL', 'RAMIREZ', MANCERA, 'aramirez', 'oEFPCa1Z1k+qV2t65a98yA==', 6, 1, 1)</v>
+      </c>
+      <c r="T6" s="1">
         <v>5</v>
-      </c>
-      <c r="S6" s="1">
-        <v>8</v>
-      </c>
-      <c r="T6" s="1" t="str">
-        <f>_xlfn.CONCAT("INSERT INTO ", Hoja2!$C$33, " (", $R$1, ", ", $S$1, ") VALUES(", R6, ", ", S6, ")")</f>
-        <v>INSERT INTO EmpleadoArea (nIdEmpleado, nIdArea) VALUES(5, 8)</v>
       </c>
       <c r="U6" s="1">
         <v>8</v>
       </c>
-      <c r="V6" s="1">
+      <c r="V6" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO ", Hoja2!$C$35, " (", $T$1, ", ", $U$1, ") VALUES(", T6, ", ", U6, ")")</f>
+        <v>INSERT INTO EmpleadoArea (nIdEmpleado, nIdArea) VALUES(5, 8)</v>
+      </c>
+      <c r="W6" s="1">
+        <v>8</v>
+      </c>
+      <c r="X6" s="1">
         <v>63</v>
       </c>
-      <c r="W6" s="1" t="str">
-        <f>_xlfn.CONCAT("INSERT INTO ", Hoja2!$C$39, " (", $U$1, ", ", $V$1, ") VALUES(", U6, ", ", V6, ")")</f>
+      <c r="Y6" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO ", Hoja2!$C$41, " (", $W$1, ", ", $X$1, ") VALUES(", W6, ", ", X6, ")")</f>
         <v>INSERT INTO AreaAplicativo (nIdArea, nIdAplicativo) VALUES(8, 63)</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>115</v>
       </c>
@@ -3808,46 +3933,49 @@
         <f>_xlfn.CONCAT("INSERT INTO ",Hoja2!$C$8, " (", $C$1, ", ", $D$1, ", ", $E$1, ", ", $F$1, ", ", $G$1, ", Estado) VALUES(", C7, ", '", D7, "', ", E7, ", '", F7, "', '", G7, "', 1)")</f>
         <v>INSERT INTO TablasDetalles (nIdTabla, Acronimo, Orden, TablaDetalle, Observaciones, Estado) VALUES(2, 'Rech', 0, 'Rechazado', '', 1)</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="I7" s="1">
+        <v>8</v>
+      </c>
+      <c r="K7" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="L7" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="K7" s="1" t="s">
+      <c r="M7" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="L7" s="1" t="s">
+      <c r="N7" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="M7" s="1" t="s">
+      <c r="O7" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="N7" s="1">
+      <c r="P7" s="1">
         <v>5</v>
       </c>
-      <c r="O7" s="1">
-        <v>0</v>
-      </c>
-      <c r="P7" s="1">
-        <v>1</v>
-      </c>
-      <c r="Q7" s="1" t="str">
-        <f>_xlfn.CONCAT("INSERT INTO ",Hoja2!$C$19, " (",$I$1, ", ", $J$1, ", ", $K$1, ", ", $L$1, ", ", $M$1, ", ", $N$1, ", ", $O$1, ", ", $P$1, ") VALUES('", I7, "', '", J7, "', ", K7, ", '", L7, "', '", M7, "', ", N7, ", ", O7, ", ", P7, ")")</f>
-        <v>INSERT INTO Empleados (sNombre, sApellido1, sApellido2, sUsuario, sContra, Orden, Root, Estado) VALUES('JACOB ADIEL', 'GARCIA', GARCIA, 'jgarcia', 'oEFPCa1Z1k+qV2t65a98yA==', 5, 0, 1)</v>
+      <c r="Q7" s="1">
+        <v>0</v>
       </c>
       <c r="R7" s="1">
+        <v>1</v>
+      </c>
+      <c r="S7" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO ",Hoja2!$C$19, " (", $I$1, ", ", $J$1, ", ",$K$1, ", ", $L$1, ", ", $M$1, ", ", $N$1, ", ", $O$1, ", ", $P$1, ", ", $Q$1, ", ", $R$1, ") VALUES(", I7, ", null, '", K7, "', '", L7, "', ", M7, ", '", N7, "', '", O7, "', ", P7, ", ", Q7, ", ", R7, ")")</f>
+        <v>INSERT INTO Empleados (nIdArea, nIdAplicativo, sNombre, sApellido1, sApellido2, sUsuario, sContra, Orden, Root, Estado) VALUES(8, null, 'JACOB ADIEL', 'GARCIA', GARCIA, 'jgarcia', 'oEFPCa1Z1k+qV2t65a98yA==', 5, 0, 1)</v>
+      </c>
+      <c r="T7" s="1">
         <v>6</v>
       </c>
-      <c r="S7" s="1">
+      <c r="U7" s="1">
         <v>8</v>
       </c>
-      <c r="T7" s="1" t="str">
-        <f>_xlfn.CONCAT("INSERT INTO ", Hoja2!$C$33, " (", $R$1, ", ", $S$1, ") VALUES(", R7, ", ", S7, ")")</f>
+      <c r="V7" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO ", Hoja2!$C$35, " (", $T$1, ", ", $U$1, ") VALUES(", T7, ", ", U7, ")")</f>
         <v>INSERT INTO EmpleadoArea (nIdEmpleado, nIdArea) VALUES(6, 8)</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>31</v>
       </c>
@@ -3872,7 +4000,7 @@
         <v>INSERT INTO TablasDetalles (nIdTabla, Acronimo, Orden, TablaDetalle, Observaciones, Estado) VALUES(2, 'CanInt', 0, 'Cancelado', '', 1)</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
       <c r="C9" s="1">
         <v>3</v>
       </c>
@@ -3890,7 +4018,7 @@
         <v>INSERT INTO TablasDetalles (nIdTabla, Acronimo, Orden, TablaDetalle, Observaciones, Estado) VALUES(3, '', 0, 'APE4', 'APE4', 1)</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
       <c r="C10" s="1">
         <v>3</v>
       </c>
@@ -3908,7 +4036,7 @@
         <v>INSERT INTO TablasDetalles (nIdTabla, Acronimo, Orden, TablaDetalle, Observaciones, Estado) VALUES(3, '', 0, 'APE1', 'APE4', 1)</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
       <c r="C11" s="1">
         <v>3</v>
       </c>
@@ -3926,7 +4054,7 @@
         <v>INSERT INTO TablasDetalles (nIdTabla, Acronimo, Orden, TablaDetalle, Observaciones, Estado) VALUES(3, '', 0, 'APE2', 'APE4', 1)</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
       <c r="C12" s="1">
         <v>3</v>
       </c>
@@ -3944,7 +4072,7 @@
         <v>INSERT INTO TablasDetalles (nIdTabla, Acronimo, Orden, TablaDetalle, Observaciones, Estado) VALUES(3, '', 0, 'Azure', 'APE4', 1)</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
       <c r="C13" s="1">
         <v>4</v>
       </c>
@@ -3962,7 +4090,7 @@
         <v>INSERT INTO TablasDetalles (nIdTabla, Acronimo, Orden, TablaDetalle, Observaciones, Estado) VALUES(4, '', 16, 'Registro RDL', 'Softtek', 1)</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
       <c r="C14" s="1">
         <v>4</v>
       </c>
@@ -3980,7 +4108,7 @@
         <v>INSERT INTO TablasDetalles (nIdTabla, Acronimo, Orden, TablaDetalle, Observaciones, Estado) VALUES(4, '', 17, 'Verificacion Desarrollo', 'RAPE', 1)</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
       <c r="C15" s="1">
         <v>4</v>
       </c>
@@ -3998,7 +4126,7 @@
         <v>INSERT INTO TablasDetalles (nIdTabla, Acronimo, Orden, TablaDetalle, Observaciones, Estado) VALUES(4, '', 18, 'Recepción Versiones', 'AVL', 1)</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
       <c r="C16" s="1">
         <v>4</v>
       </c>
@@ -4867,92 +4995,257 @@
     </row>
     <row r="65" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C65" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E65" s="1">
-        <v>12</v>
+        <v>404</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="G65" s="1" t="s">
-        <v>130</v>
+        <v>177</v>
       </c>
       <c r="H65" s="1" t="str">
         <f>_xlfn.CONCAT("INSERT INTO ",Hoja2!$C$8, " (", $C$1, ", ", $D$1, ", ", $E$1, ", ", $F$1, ", ", $G$1, ", Estado) VALUES(", C65, ", '", D65, "', ", E65, ", '", F65, "', '", G65, "', 1)")</f>
-        <v>INSERT INTO TablasDetalles (nIdTabla, Acronimo, Orden, TablaDetalle, Observaciones, Estado) VALUES(7, '', 12, 'dyp_pp_cun-web', 'https://gitlab.sat.gob.mx/avl/[REP]|https://gitlab.sat.gob.mx/avl/[REP]|http://18.144.132.20/proyectos/sat/sdma6/ape1/dyp/[REP]/-/tree/main/Continuidad%20Operativa/Incidencias/RMA-[RMA]/[PAQ]', 1)</v>
+        <v>INSERT INTO TablasDetalles (nIdTabla, Acronimo, Orden, TablaDetalle, Observaciones, Estado) VALUES(6, '', 404, 'FORMA R15', '', 1)</v>
       </c>
     </row>
     <row r="66" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C66" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E66" s="1">
-        <v>105</v>
+        <v>81</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="G66" s="1" t="s">
-        <v>130</v>
+        <v>178</v>
       </c>
       <c r="H66" s="1" t="str">
         <f>_xlfn.CONCAT("INSERT INTO ",Hoja2!$C$8, " (", $C$1, ", ", $D$1, ", ", $E$1, ", ", $F$1, ", ", $G$1, ", Estado) VALUES(", C66, ", '", D66, "', ", E66, ", '", F66, "', '", G66, "', 1)")</f>
-        <v>INSERT INTO TablasDetalles (nIdTabla, Acronimo, Orden, TablaDetalle, Observaciones, Estado) VALUES(7, '', 105, 'dyp_lda_nepe', 'https://gitlab.sat.gob.mx/avl/[REP]|https://gitlab.sat.gob.mx/avl/[REP]|http://18.144.132.20/proyectos/sat/sdma6/ape1/dyp/[REP]/-/tree/main/Continuidad%20Operativa/Incidencias/RMA-[RMA]/[PAQ]', 1)</v>
+        <v>INSERT INTO TablasDetalles (nIdTabla, Acronimo, Orden, TablaDetalle, Observaciones, Estado) VALUES(6, '', 81, 'CONTABILIDAD NEPE', '', 1)</v>
       </c>
     </row>
     <row r="67" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C67" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E67" s="1">
-        <v>355</v>
+        <v>417</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="G67" s="1" t="s">
-        <v>134</v>
+        <v>179</v>
       </c>
       <c r="H67" s="1" t="str">
         <f>_xlfn.CONCAT("INSERT INTO ",Hoja2!$C$8, " (", $C$1, ", ", $D$1, ", ", $E$1, ", ", $F$1, ", ", $G$1, ", Estado) VALUES(", C67, ", '", D67, "', ", E67, ", '", F67, "', '", G67, "', 1)")</f>
-        <v>INSERT INTO TablasDetalles (nIdTabla, Acronimo, Orden, TablaDetalle, Observaciones, Estado) VALUES(7, '', 355, 'dyp_pp_diot', 'https://gitlab.sat.gob.mx/avl/[REP]|http://18.144.132.20/proyectos/sat/sdma6/ape1/dyp/[REP]/-/tree/main/Continuidad%20Operativa/Incidencias/RMA-[RMA]/[PAQ]', 1)</v>
+        <v>INSERT INTO TablasDetalles (nIdTabla, Acronimo, Orden, TablaDetalle, Observaciones, Estado) VALUES(6, '', 417, 'VALIDADOR DE INTERESES', '', 1)</v>
       </c>
     </row>
     <row r="68" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C68" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E68" s="1">
-        <v>104</v>
+        <v>416</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="G68" s="1" t="s">
-        <v>130</v>
+        <v>180</v>
       </c>
       <c r="H68" s="1" t="str">
         <f>_xlfn.CONCAT("INSERT INTO ",Hoja2!$C$8, " (", $C$1, ", ", $D$1, ", ", $E$1, ", ", $F$1, ", ", $G$1, ", Estado) VALUES(", C68, ", '", D68, "', ", E68, ", '", F68, "', '", G68, "', 1)")</f>
-        <v>INSERT INTO TablasDetalles (nIdTabla, Acronimo, Orden, TablaDetalle, Observaciones, Estado) VALUES(7, '', 104, 'dyp_lda_modelo', 'https://gitlab.sat.gob.mx/avl/[REP]|https://gitlab.sat.gob.mx/avl/[REP]|http://18.144.132.20/proyectos/sat/sdma6/ape1/dyp/[REP]/-/tree/main/Continuidad%20Operativa/Incidencias/RMA-[RMA]/[PAQ]', 1)</v>
+        <v>INSERT INTO TablasDetalles (nIdTabla, Acronimo, Orden, TablaDetalle, Observaciones, Estado) VALUES(6, '', 416, 'VALIDADOR DE FIDEICOMISOS', '', 1)</v>
       </c>
     </row>
     <row r="69" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C69" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E69" s="1">
-        <v>382</v>
+        <v>125</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="G69" s="1" t="s">
-        <v>130</v>
+        <v>181</v>
       </c>
       <c r="H69" s="1" t="str">
         <f>_xlfn.CONCAT("INSERT INTO ",Hoja2!$C$8, " (", $C$1, ", ", $D$1, ", ", $E$1, ", ", $F$1, ", ", $G$1, ", Estado) VALUES(", C69, ", '", D69, "', ", E69, ", '", F69, "', '", G69, "', 1)")</f>
+        <v>INSERT INTO TablasDetalles (nIdTabla, Acronimo, Orden, TablaDetalle, Observaciones, Estado) VALUES(6, '', 125, 'FORMA 35 DECLARACION INFORMATIVA', '', 1)</v>
+      </c>
+    </row>
+    <row r="70" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C70" s="1">
+        <v>7</v>
+      </c>
+      <c r="E70" s="1">
+        <v>12</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="G70" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="H70" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO ",Hoja2!$C$8, " (", $C$1, ", ", $D$1, ", ", $E$1, ", ", $F$1, ", ", $G$1, ", Estado) VALUES(", C70, ", '", D70, "', ", E70, ", '", F70, "', '", G70, "', 1)")</f>
+        <v>INSERT INTO TablasDetalles (nIdTabla, Acronimo, Orden, TablaDetalle, Observaciones, Estado) VALUES(7, '', 12, 'dyp_pp_cun-web', 'https://gitlab.sat.gob.mx/avl/[REP]|https://gitlab.sat.gob.mx/avl/[REP]|http://18.144.132.20/proyectos/sat/sdma6/ape1/dyp/[REP]/-/tree/main/Continuidad%20Operativa/Incidencias/RMA-[RMA]/[PAQ]', 1)</v>
+      </c>
+    </row>
+    <row r="71" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C71" s="1">
+        <v>7</v>
+      </c>
+      <c r="E71" s="1">
+        <v>105</v>
+      </c>
+      <c r="F71" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="G71" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="H71" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO ",Hoja2!$C$8, " (", $C$1, ", ", $D$1, ", ", $E$1, ", ", $F$1, ", ", $G$1, ", Estado) VALUES(", C71, ", '", D71, "', ", E71, ", '", F71, "', '", G71, "', 1)")</f>
+        <v>INSERT INTO TablasDetalles (nIdTabla, Acronimo, Orden, TablaDetalle, Observaciones, Estado) VALUES(7, '', 105, 'dyp_lda_nepe', 'https://gitlab.sat.gob.mx/avl/[REP]|https://gitlab.sat.gob.mx/avl/[REP]|http://18.144.132.20/proyectos/sat/sdma6/ape1/dyp/[REP]/-/tree/main/Continuidad%20Operativa/Incidencias/RMA-[RMA]/[PAQ]', 1)</v>
+      </c>
+    </row>
+    <row r="72" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C72" s="1">
+        <v>7</v>
+      </c>
+      <c r="E72" s="1">
+        <v>355</v>
+      </c>
+      <c r="F72" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="G72" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="H72" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO ",Hoja2!$C$8, " (", $C$1, ", ", $D$1, ", ", $E$1, ", ", $F$1, ", ", $G$1, ", Estado) VALUES(", C72, ", '", D72, "', ", E72, ", '", F72, "', '", G72, "', 1)")</f>
+        <v>INSERT INTO TablasDetalles (nIdTabla, Acronimo, Orden, TablaDetalle, Observaciones, Estado) VALUES(7, '', 355, 'dyp_pp_diot', 'https://gitlab.sat.gob.mx/avl/[REP]|http://18.144.132.20/proyectos/sat/sdma6/ape1/dyp/[REP]/-/tree/main/Continuidad%20Operativa/Incidencias/RMA-[RMA]/[PAQ]', 1)</v>
+      </c>
+    </row>
+    <row r="73" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C73" s="1">
+        <v>7</v>
+      </c>
+      <c r="E73" s="1">
+        <v>104</v>
+      </c>
+      <c r="F73" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="G73" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="H73" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO ",Hoja2!$C$8, " (", $C$1, ", ", $D$1, ", ", $E$1, ", ", $F$1, ", ", $G$1, ", Estado) VALUES(", C73, ", '", D73, "', ", E73, ", '", F73, "', '", G73, "', 1)")</f>
+        <v>INSERT INTO TablasDetalles (nIdTabla, Acronimo, Orden, TablaDetalle, Observaciones, Estado) VALUES(7, '', 104, 'dyp_lda_modelo', 'https://gitlab.sat.gob.mx/avl/[REP]|https://gitlab.sat.gob.mx/avl/[REP]|http://18.144.132.20/proyectos/sat/sdma6/ape1/dyp/[REP]/-/tree/main/Continuidad%20Operativa/Incidencias/RMA-[RMA]/[PAQ]', 1)</v>
+      </c>
+    </row>
+    <row r="74" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C74" s="1">
+        <v>7</v>
+      </c>
+      <c r="E74" s="1">
+        <v>382</v>
+      </c>
+      <c r="F74" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="G74" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="H74" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO ",Hoja2!$C$8, " (", $C$1, ", ", $D$1, ", ", $E$1, ", ", $F$1, ", ", $G$1, ", Estado) VALUES(", C74, ", '", D74, "', ", E74, ", '", F74, "', '", G74, "', 1)")</f>
         <v>INSERT INTO TablasDetalles (nIdTabla, Acronimo, Orden, TablaDetalle, Observaciones, Estado) VALUES(7, '', 382, 'dyp_pp_dec_ide', 'https://gitlab.sat.gob.mx/avl/[REP]|https://gitlab.sat.gob.mx/avl/[REP]|http://18.144.132.20/proyectos/sat/sdma6/ape1/dyp/[REP]/-/tree/main/Continuidad%20Operativa/Incidencias/RMA-[RMA]/[PAQ]', 1)</v>
+      </c>
+    </row>
+    <row r="75" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C75" s="1">
+        <v>7</v>
+      </c>
+      <c r="E75" s="1">
+        <v>404</v>
+      </c>
+      <c r="F75" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="G75" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="H75" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO ",Hoja2!$C$8, " (", $C$1, ", ", $D$1, ", ", $E$1, ", ", $F$1, ", ", $G$1, ", Estado) VALUES(", C75, ", '", D75, "', ", E75, ", '", F75, "', '", G75, "', 1)")</f>
+        <v>INSERT INTO TablasDetalles (nIdTabla, Acronimo, Orden, TablaDetalle, Observaciones, Estado) VALUES(7, '', 404, 'dyp_pp_forma_r15', 'https://gitlab.sat.gob.mx/avl/[REP]|https://gitlab.sat.gob.mx/avl/[REP]|http://18.144.132.20/proyectos/sat/sdma6/ape1/dyp/[REP]/-/tree/main/Continuidad%20Operativa/Incidencias/RMA-[RMA]/[PAQ]', 1)</v>
+      </c>
+    </row>
+    <row r="76" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C76" s="1">
+        <v>7</v>
+      </c>
+      <c r="E76" s="1">
+        <v>81</v>
+      </c>
+      <c r="F76" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="G76" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="H76" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO ",Hoja2!$C$8, " (", $C$1, ", ", $D$1, ", ", $E$1, ", ", $F$1, ", ", $G$1, ", Estado) VALUES(", C76, ", '", D76, "', ", E76, ", '", F76, "', '", G76, "', 1)")</f>
+        <v>INSERT INTO TablasDetalles (nIdTabla, Acronimo, Orden, TablaDetalle, Observaciones, Estado) VALUES(7, '', 81, 'rc_contabilidad_nepe', 'https://gitlab.sat.gob.mx/avl/[REP]|https://gitlab.sat.gob.mx/avl/[REP]|http://18.144.132.20/proyectos/sat/sdma6/ape1/dyp/[REP]/-/tree/main/Continuidad%20Operativa/Incidencias/RMA-[RMA]/[PAQ]', 1)</v>
+      </c>
+    </row>
+    <row r="77" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C77" s="1">
+        <v>7</v>
+      </c>
+      <c r="E77" s="1">
+        <v>417</v>
+      </c>
+      <c r="F77" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="G77" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="H77" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO ",Hoja2!$C$8, " (", $C$1, ", ", $D$1, ", ", $E$1, ", ", $F$1, ", ", $G$1, ", Estado) VALUES(", C77, ", '", D77, "', ", E77, ", '", F77, "', '", G77, "', 1)")</f>
+        <v>INSERT INTO TablasDetalles (nIdTabla, Acronimo, Orden, TablaDetalle, Observaciones, Estado) VALUES(7, '', 417, 'dyp_lda_validador_de_intereses', 'https://gitlab.sat.gob.mx/avl/[REP]|https://gitlab.sat.gob.mx/avl/[REP]|http://18.144.132.20/proyectos/sat/sdma6/ape1/dyp/[REP]/-/tree/main/Continuidad%20Operativa/Incidencias/RMA-[RMA]/[PAQ]', 1)</v>
+      </c>
+    </row>
+    <row r="78" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C78" s="1">
+        <v>7</v>
+      </c>
+      <c r="E78" s="1">
+        <v>416</v>
+      </c>
+      <c r="F78" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="G78" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="H78" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO ",Hoja2!$C$8, " (", $C$1, ", ", $D$1, ", ", $E$1, ", ", $F$1, ", ", $G$1, ", Estado) VALUES(", C78, ", '", D78, "', ", E78, ", '", F78, "', '", G78, "', 1)")</f>
+        <v>INSERT INTO TablasDetalles (nIdTabla, Acronimo, Orden, TablaDetalle, Observaciones, Estado) VALUES(7, '', 416, 'dyp_lda_validador_de_fideicomisos', 'https://gitlab.sat.gob.mx/avl/[REP]|https://gitlab.sat.gob.mx/avl/[REP]|http://18.144.132.20/proyectos/sat/sdma6/ape1/dyp/[REP]/-/tree/main/Continuidad%20Operativa/Incidencias/RMA-[RMA]/[PAQ]', 1)</v>
+      </c>
+    </row>
+    <row r="79" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C79" s="1">
+        <v>7</v>
+      </c>
+      <c r="E79" s="1">
+        <v>125</v>
+      </c>
+      <c r="F79" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="G79" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="H79" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO ",Hoja2!$C$8, " (", $C$1, ", ", $D$1, ", ", $E$1, ", ", $F$1, ", ", $G$1, ", Estado) VALUES(", C79, ", '", D79, "', ", E79, ", '", F79, "', '", G79, "', 1)")</f>
+        <v>INSERT INTO TablasDetalles (nIdTabla, Acronimo, Orden, TablaDetalle, Observaciones, Estado) VALUES(7, '', 125, 'dyp_pp_forma_35', 'https://gitlab.sat.gob.mx/avl/[REP]|https://gitlab.sat.gob.mx/avl/[REP]|http://18.144.132.20/proyectos/sat/sdma6/ape1/dyp/[REP]/-/tree/main/Continuidad%20Operativa/Incidencias/RMA-[RMA]/[PAQ]', 1)</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se suben componentes de modificaciones al proyecto de MonitorRMA.
</commit_message>
<xml_diff>
--- a/MonitorRMA/BaseDatos/Estructura.xlsx
+++ b/MonitorRMA/BaseDatos/Estructura.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DatosPersonales\Personales\Repositorio\GitHub\DesarrolloARM\MonitorRMA\BaseDatos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30425FBC-424E-4786-93C2-88188E7D5DB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19DFA5F0-A29E-4C0A-8A51-120D09637794}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="10845" activeTab="1" xr2:uid="{010BB1C2-CC3F-48D4-9CA6-4C5256A0A30C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="1" xr2:uid="{010BB1C2-CC3F-48D4-9CA6-4C5256A0A30C}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja2" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="191">
   <si>
     <t>RMA</t>
   </si>
@@ -120,9 +120,6 @@
     <t>Tipos Requerimientos</t>
   </si>
   <si>
-    <t>POL</t>
-  </si>
-  <si>
     <t>DatosPaquete</t>
   </si>
   <si>
@@ -598,6 +595,21 @@
   </si>
   <si>
     <t>dyp_pp_forma_35</t>
+  </si>
+  <si>
+    <t>Mantenimiento Menor</t>
+  </si>
+  <si>
+    <t>MMay</t>
+  </si>
+  <si>
+    <t>Servicio</t>
+  </si>
+  <si>
+    <t>Mmen</t>
+  </si>
+  <si>
+    <t>Mantenimiento Mayor</t>
   </si>
 </sst>
 </file>
@@ -1008,7 +1020,7 @@
         <v>CREATE TABLE Tablas(</v>
       </c>
       <c r="J1" s="1" t="str">
-        <f t="shared" ref="J1:J66" si="1">IF(I1="",_xlfn.CONCAT("	", A1," ",B1,IF(C1&gt;0,_xlfn.CONCAT("(",C1,")"),""),IF(D1=1," NOT NULL"," NULL"),IF(F1=1," IDENTITY(1,1)",""),IF(E1=1," PRIMARY KEY",""),IF(G1&lt;&gt;"",_xlfn.CONCAT(" ",G1),""),IF(I2=0,")
+        <f t="shared" ref="J1:J20" si="1">IF(I1="",_xlfn.CONCAT("	", A1," ",B1,IF(C1&gt;0,_xlfn.CONCAT("(",C1,")"),""),IF(D1=1," NOT NULL"," NULL"),IF(F1=1," IDENTITY(1,1)",""),IF(E1=1," PRIMARY KEY",""),IF(G1&lt;&gt;"",_xlfn.CONCAT(" ",G1),""),IF(I2=0,")
 GO",", ")),IF(I1=1,_xlfn.CONCAT(B1,", "), ""))</f>
         <v/>
       </c>
@@ -1113,10 +1125,10 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>47</v>
       </c>
       <c r="C5" s="4">
         <v>0</v>
@@ -1289,7 +1301,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>5</v>
@@ -1315,7 +1327,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>3</v>
@@ -1367,7 +1379,7 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>5</v>
@@ -1393,10 +1405,10 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>47</v>
       </c>
       <c r="C16" s="4">
         <v>0</v>
@@ -1453,7 +1465,7 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C19" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
@@ -1507,7 +1519,7 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>3</v>
@@ -1540,7 +1552,7 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>3</v>
@@ -1569,7 +1581,7 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>3</v>
@@ -1597,7 +1609,7 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>5</v>
@@ -1623,7 +1635,7 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>5</v>
@@ -1649,7 +1661,7 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>5</v>
@@ -1675,7 +1687,7 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>5</v>
@@ -1701,7 +1713,7 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>5</v>
@@ -1727,7 +1739,7 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>3</v>
@@ -1753,10 +1765,10 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C30" s="4">
         <v>0</v>
@@ -1779,10 +1791,10 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>47</v>
       </c>
       <c r="C31" s="4">
         <v>0</v>
@@ -1858,7 +1870,7 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C35" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="I35" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1910,7 +1922,7 @@
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>3</v>
@@ -1944,7 +1956,7 @@
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>3</v>
@@ -2010,7 +2022,7 @@
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C41" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D41" s="4"/>
       <c r="I41" s="1" t="str">
@@ -2063,7 +2075,7 @@
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>3</v>
@@ -2097,7 +2109,7 @@
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>3</v>
@@ -2278,7 +2290,7 @@
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>3</v>
@@ -2308,7 +2320,7 @@
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>3</v>
@@ -2338,7 +2350,7 @@
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>3</v>
@@ -2498,7 +2510,7 @@
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>5</v>
@@ -2524,10 +2536,10 @@
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C60" s="1">
         <v>0</v>
@@ -2550,10 +2562,10 @@
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C61" s="1">
         <v>0</v>
@@ -2578,7 +2590,7 @@
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>5</v>
@@ -2636,7 +2648,7 @@
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C65" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I65" s="1" t="str">
         <f t="shared" si="2"/>
@@ -2688,7 +2700,7 @@
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>3</v>
@@ -2750,7 +2762,7 @@
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>3</v>
@@ -2780,7 +2792,7 @@
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>4</v>
@@ -2806,7 +2818,7 @@
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>5</v>
@@ -2832,7 +2844,7 @@
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>5</v>
@@ -2884,7 +2896,7 @@
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>5</v>
@@ -2912,7 +2924,7 @@
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>5</v>
@@ -2970,7 +2982,7 @@
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C78" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I78" s="1" t="str">
         <f t="shared" si="5"/>
@@ -3022,7 +3034,7 @@
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>3</v>
@@ -3054,7 +3066,7 @@
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>3</v>
@@ -3084,7 +3096,7 @@
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>3</v>
@@ -3110,7 +3122,7 @@
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>5</v>
@@ -3133,10 +3145,10 @@
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C84" s="1">
         <v>0</v>
@@ -3156,10 +3168,10 @@
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C85" s="1">
         <v>0</v>
@@ -3181,10 +3193,10 @@
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C86" s="1">
         <v>0</v>
@@ -3205,10 +3217,10 @@
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C87" s="1">
         <v>0</v>
@@ -3244,7 +3256,7 @@
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C89" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I89" s="1" t="str">
         <f t="shared" si="5"/>
@@ -3296,7 +3308,7 @@
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B91" s="1" t="s">
         <v>3</v>
@@ -3360,7 +3372,7 @@
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B93" s="1" t="s">
         <v>3</v>
@@ -3440,10 +3452,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E7C2D72-1FAE-4DEA-8254-172C45BBECDF}">
-  <dimension ref="A1:Y79"/>
+  <dimension ref="A1:Y81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="Y2" sqref="Y2:Y6"/>
+    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2:H81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -3475,58 +3487,58 @@
         <v>16</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>45</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>19</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="Q1" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>46</v>
-      </c>
       <c r="T1" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="W1" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.2">
@@ -3557,19 +3569,19 @@
         <v>8</v>
       </c>
       <c r="K2" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="L2" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="M2" s="1" t="s">
-        <v>146</v>
-      </c>
       <c r="N2" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="P2" s="1">
         <v>3</v>
@@ -3607,7 +3619,7 @@
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B3" s="1" t="str">
         <f>_xlfn.CONCAT("INSERT INTO ", Hoja2!$C$1, " (", $A$1, ", Estado) VALUES('", A3, "', 1)")</f>
@@ -3617,35 +3629,35 @@
         <v>1</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>27</v>
+        <v>189</v>
       </c>
       <c r="E3" s="1">
         <v>0</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>27</v>
+        <v>186</v>
       </c>
       <c r="H3" s="1" t="str">
         <f>_xlfn.CONCAT("INSERT INTO ",Hoja2!$C$8, " (", $C$1, ", ", $D$1, ", ", $E$1, ", ", $F$1, ", ", $G$1, ", Estado) VALUES(", C3, ", '", D3, "', ", E3, ", '", F3, "', '", G3, "', 1)")</f>
-        <v>INSERT INTO TablasDetalles (nIdTabla, Acronimo, Orden, TablaDetalle, Observaciones, Estado) VALUES(1, 'POL', 0, 'POL', '', 1)</v>
+        <v>INSERT INTO TablasDetalles (nIdTabla, Acronimo, Orden, TablaDetalle, Observaciones, Estado) VALUES(1, 'Mmen', 0, 'Mantenimiento Menor', '', 1)</v>
       </c>
       <c r="I3" s="1">
         <v>8</v>
       </c>
       <c r="K3" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="L3" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="M3" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="M3" s="1" t="s">
-        <v>149</v>
-      </c>
       <c r="N3" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="P3" s="1">
         <v>4</v>
@@ -3683,7 +3695,7 @@
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B4" s="1" t="str">
         <f>_xlfn.CONCAT("INSERT INTO ", Hoja2!$C$1, " (", $A$1, ", Estado) VALUES('", A4, "', 1)")</f>
@@ -3693,13 +3705,13 @@
         <v>2</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E4" s="1">
         <v>0</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H4" s="1" t="str">
         <f>_xlfn.CONCAT("INSERT INTO ",Hoja2!$C$8, " (", $C$1, ", ", $D$1, ", ", $E$1, ", ", $F$1, ", ", $G$1, ", Estado) VALUES(", C4, ", '", D4, "', ", E4, ", '", F4, "', '", G4, "', 1)")</f>
@@ -3709,19 +3721,19 @@
         <v>8</v>
       </c>
       <c r="K4" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="M4" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="L4" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>151</v>
-      </c>
       <c r="N4" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="P4" s="1">
         <v>1</v>
@@ -3759,7 +3771,7 @@
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B5" s="1" t="str">
         <f>_xlfn.CONCAT("INSERT INTO ", Hoja2!$C$1, " (", $A$1, ", Estado) VALUES('", A5, "', 1)")</f>
@@ -3769,13 +3781,13 @@
         <v>2</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E5" s="1">
         <v>0</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H5" s="1" t="str">
         <f>_xlfn.CONCAT("INSERT INTO ",Hoja2!$C$8, " (", $C$1, ", ", $D$1, ", ", $E$1, ", ", $F$1, ", ", $G$1, ", Estado) VALUES(", C5, ", '", D5, "', ", E5, ", '", F5, "', '", G5, "', 1)")</f>
@@ -3785,19 +3797,19 @@
         <v>8</v>
       </c>
       <c r="K5" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="L5" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="L5" s="1" t="s">
+      <c r="M5" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="M5" s="1" t="s">
-        <v>154</v>
-      </c>
       <c r="N5" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="P5" s="1">
         <v>2</v>
@@ -3835,7 +3847,7 @@
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B6" s="1" t="str">
         <f>_xlfn.CONCAT("INSERT INTO ", Hoja2!$C$1, " (", $A$1, ", Estado) VALUES('", A6, "', 1)")</f>
@@ -3845,13 +3857,13 @@
         <v>2</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E6" s="1">
         <v>0</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H6" s="1" t="str">
         <f>_xlfn.CONCAT("INSERT INTO ",Hoja2!$C$8, " (", $C$1, ", ", $D$1, ", ", $E$1, ", ", $F$1, ", ", $G$1, ", Estado) VALUES(", C6, ", '", D6, "', ", E6, ", '", F6, "', '", G6, "', 1)")</f>
@@ -3861,19 +3873,19 @@
         <v>8</v>
       </c>
       <c r="K6" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="L6" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="L6" s="1" t="s">
+      <c r="M6" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="M6" s="1" t="s">
-        <v>157</v>
-      </c>
       <c r="N6" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="P6" s="1">
         <v>6</v>
@@ -3911,7 +3923,7 @@
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B7" s="1" t="str">
         <f>_xlfn.CONCAT("INSERT INTO ", Hoja2!$C$1, " (", $A$1, ", Estado) VALUES('", A7, "', 1)")</f>
@@ -3921,13 +3933,13 @@
         <v>2</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E7" s="1">
         <v>0</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H7" s="1" t="str">
         <f>_xlfn.CONCAT("INSERT INTO ",Hoja2!$C$8, " (", $C$1, ", ", $D$1, ", ", $E$1, ", ", $F$1, ", ", $G$1, ", Estado) VALUES(", C7, ", '", D7, "', ", E7, ", '", F7, "', '", G7, "', 1)")</f>
@@ -3937,19 +3949,19 @@
         <v>8</v>
       </c>
       <c r="K7" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="L7" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="L7" s="1" t="s">
-        <v>159</v>
-      </c>
       <c r="M7" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="P7" s="1">
         <v>5</v>
@@ -3977,7 +3989,7 @@
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B8" s="1" t="str">
         <f>_xlfn.CONCAT("INSERT INTO ", Hoja2!$C$1, " (", $A$1, ", Estado) VALUES('", A8, "', 1)")</f>
@@ -3987,18 +3999,28 @@
         <v>2</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E8" s="1">
         <v>0</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H8" s="1" t="str">
         <f>_xlfn.CONCAT("INSERT INTO ",Hoja2!$C$8, " (", $C$1, ", ", $D$1, ", ", $E$1, ", ", $F$1, ", ", $G$1, ", Estado) VALUES(", C8, ", '", D8, "', ", E8, ", '", F8, "', '", G8, "', 1)")</f>
         <v>INSERT INTO TablasDetalles (nIdTabla, Acronimo, Orden, TablaDetalle, Observaciones, Estado) VALUES(2, 'CanInt', 0, 'Cancelado', '', 1)</v>
       </c>
+      <c r="T8" s="1">
+        <v>6</v>
+      </c>
+      <c r="U8" s="1">
+        <v>9</v>
+      </c>
+      <c r="V8" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO ", Hoja2!$C$35, " (", $T$1, ", ", $U$1, ") VALUES(", T8, ", ", U8, ")")</f>
+        <v>INSERT INTO EmpleadoArea (nIdEmpleado, nIdArea) VALUES(6, 9)</v>
+      </c>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.2">
       <c r="C9" s="1">
@@ -4008,10 +4030,10 @@
         <v>0</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H9" s="1" t="str">
         <f>_xlfn.CONCAT("INSERT INTO ",Hoja2!$C$8, " (", $C$1, ", ", $D$1, ", ", $E$1, ", ", $F$1, ", ", $G$1, ", Estado) VALUES(", C9, ", '", D9, "', ", E9, ", '", F9, "', '", G9, "', 1)")</f>
@@ -4026,10 +4048,10 @@
         <v>0</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H10" s="1" t="str">
         <f>_xlfn.CONCAT("INSERT INTO ",Hoja2!$C$8, " (", $C$1, ", ", $D$1, ", ", $E$1, ", ", $F$1, ", ", $G$1, ", Estado) VALUES(", C10, ", '", D10, "', ", E10, ", '", F10, "', '", G10, "', 1)")</f>
@@ -4044,10 +4066,10 @@
         <v>0</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H11" s="1" t="str">
         <f>_xlfn.CONCAT("INSERT INTO ",Hoja2!$C$8, " (", $C$1, ", ", $D$1, ", ", $E$1, ", ", $F$1, ", ", $G$1, ", Estado) VALUES(", C11, ", '", D11, "', ", E11, ", '", F11, "', '", G11, "', 1)")</f>
@@ -4062,10 +4084,10 @@
         <v>0</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H12" s="1" t="str">
         <f>_xlfn.CONCAT("INSERT INTO ",Hoja2!$C$8, " (", $C$1, ", ", $D$1, ", ", $E$1, ", ", $F$1, ", ", $G$1, ", Estado) VALUES(", C12, ", '", D12, "', ", E12, ", '", F12, "', '", G12, "', 1)")</f>
@@ -4080,10 +4102,10 @@
         <v>16</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H13" s="1" t="str">
         <f>_xlfn.CONCAT("INSERT INTO ",Hoja2!$C$8, " (", $C$1, ", ", $D$1, ", ", $E$1, ", ", $F$1, ", ", $G$1, ", Estado) VALUES(", C13, ", '", D13, "', ", E13, ", '", F13, "', '", G13, "', 1)")</f>
@@ -4098,10 +4120,10 @@
         <v>17</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H14" s="1" t="str">
         <f>_xlfn.CONCAT("INSERT INTO ",Hoja2!$C$8, " (", $C$1, ", ", $D$1, ", ", $E$1, ", ", $F$1, ", ", $G$1, ", Estado) VALUES(", C14, ", '", D14, "', ", E14, ", '", F14, "', '", G14, "', 1)")</f>
@@ -4116,10 +4138,10 @@
         <v>18</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H15" s="1" t="str">
         <f>_xlfn.CONCAT("INSERT INTO ",Hoja2!$C$8, " (", $C$1, ", ", $D$1, ", ", $E$1, ", ", $F$1, ", ", $G$1, ", Estado) VALUES(", C15, ", '", D15, "', ", E15, ", '", F15, "', '", G15, "', 1)")</f>
@@ -4134,10 +4156,10 @@
         <v>19</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H16" s="1" t="str">
         <f>_xlfn.CONCAT("INSERT INTO ",Hoja2!$C$8, " (", $C$1, ", ", $D$1, ", ", $E$1, ", ", $F$1, ", ", $G$1, ", Estado) VALUES(", C16, ", '", D16, "', ", E16, ", '", F16, "', '", G16, "', 1)")</f>
@@ -4152,10 +4174,10 @@
         <v>21</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H17" s="1" t="str">
         <f>_xlfn.CONCAT("INSERT INTO ",Hoja2!$C$8, " (", $C$1, ", ", $D$1, ", ", $E$1, ", ", $F$1, ", ", $G$1, ", Estado) VALUES(", C17, ", '", D17, "', ", E17, ", '", F17, "', '", G17, "', 1)")</f>
@@ -4170,10 +4192,10 @@
         <v>23</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H18" s="1" t="str">
         <f>_xlfn.CONCAT("INSERT INTO ",Hoja2!$C$8, " (", $C$1, ", ", $D$1, ", ", $E$1, ", ", $F$1, ", ", $G$1, ", Estado) VALUES(", C18, ", '", D18, "', ", E18, ", '", F18, "', '", G18, "', 1)")</f>
@@ -4188,10 +4210,10 @@
         <v>31</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H19" s="1" t="str">
         <f>_xlfn.CONCAT("INSERT INTO ",Hoja2!$C$8, " (", $C$1, ", ", $D$1, ", ", $E$1, ", ", $F$1, ", ", $G$1, ", Estado) VALUES(", C19, ", '", D19, "', ", E19, ", '", F19, "', '", G19, "', 1)")</f>
@@ -4206,10 +4228,10 @@
         <v>38</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H20" s="1" t="str">
         <f>_xlfn.CONCAT("INSERT INTO ",Hoja2!$C$8, " (", $C$1, ", ", $D$1, ", ", $E$1, ", ", $F$1, ", ", $G$1, ", Estado) VALUES(", C20, ", '", D20, "', ", E20, ", '", F20, "', '", G20, "', 1)")</f>
@@ -4224,10 +4246,10 @@
         <v>49</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H21" s="1" t="str">
         <f>_xlfn.CONCAT("INSERT INTO ",Hoja2!$C$8, " (", $C$1, ", ", $D$1, ", ", $E$1, ", ", $F$1, ", ", $G$1, ", Estado) VALUES(", C21, ", '", D21, "', ", E21, ", '", F21, "', '", G21, "', 1)")</f>
@@ -4242,10 +4264,10 @@
         <v>55</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H22" s="1" t="str">
         <f>_xlfn.CONCAT("INSERT INTO ",Hoja2!$C$8, " (", $C$1, ", ", $D$1, ", ", $E$1, ", ", $F$1, ", ", $G$1, ", Estado) VALUES(", C22, ", '", D22, "', ", E22, ", '", F22, "', '", G22, "', 1)")</f>
@@ -4260,10 +4282,10 @@
         <v>91</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H23" s="1" t="str">
         <f>_xlfn.CONCAT("INSERT INTO ",Hoja2!$C$8, " (", $C$1, ", ", $D$1, ", ", $E$1, ", ", $F$1, ", ", $G$1, ", Estado) VALUES(", C23, ", '", D23, "', ", E23, ", '", F23, "', '", G23, "', 1)")</f>
@@ -4278,10 +4300,10 @@
         <v>92</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H24" s="1" t="str">
         <f>_xlfn.CONCAT("INSERT INTO ",Hoja2!$C$8, " (", $C$1, ", ", $D$1, ", ", $E$1, ", ", $F$1, ", ", $G$1, ", Estado) VALUES(", C24, ", '", D24, "', ", E24, ", '", F24, "', '", G24, "', 1)")</f>
@@ -4296,10 +4318,10 @@
         <v>93</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H25" s="1" t="str">
         <f>_xlfn.CONCAT("INSERT INTO ",Hoja2!$C$8, " (", $C$1, ", ", $D$1, ", ", $E$1, ", ", $F$1, ", ", $G$1, ", Estado) VALUES(", C25, ", '", D25, "', ", E25, ", '", F25, "', '", G25, "', 1)")</f>
@@ -4314,10 +4336,10 @@
         <v>98</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H26" s="1" t="str">
         <f>_xlfn.CONCAT("INSERT INTO ",Hoja2!$C$8, " (", $C$1, ", ", $D$1, ", ", $E$1, ", ", $F$1, ", ", $G$1, ", Estado) VALUES(", C26, ", '", D26, "', ", E26, ", '", F26, "', '", G26, "', 1)")</f>
@@ -4332,10 +4354,10 @@
         <v>100</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H27" s="1" t="str">
         <f>_xlfn.CONCAT("INSERT INTO ",Hoja2!$C$8, " (", $C$1, ", ", $D$1, ", ", $E$1, ", ", $F$1, ", ", $G$1, ", Estado) VALUES(", C27, ", '", D27, "', ", E27, ", '", F27, "', '", G27, "', 1)")</f>
@@ -4350,10 +4372,10 @@
         <v>127</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H28" s="1" t="str">
         <f>_xlfn.CONCAT("INSERT INTO ",Hoja2!$C$8, " (", $C$1, ", ", $D$1, ", ", $E$1, ", ", $F$1, ", ", $G$1, ", Estado) VALUES(", C28, ", '", D28, "', ", E28, ", '", F28, "', '", G28, "', 1)")</f>
@@ -4368,10 +4390,10 @@
         <v>130</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H29" s="1" t="str">
         <f>_xlfn.CONCAT("INSERT INTO ",Hoja2!$C$8, " (", $C$1, ", ", $D$1, ", ", $E$1, ", ", $F$1, ", ", $G$1, ", Estado) VALUES(", C29, ", '", D29, "', ", E29, ", '", F29, "', '", G29, "', 1)")</f>
@@ -4386,10 +4408,10 @@
         <v>131</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H30" s="1" t="str">
         <f>_xlfn.CONCAT("INSERT INTO ",Hoja2!$C$8, " (", $C$1, ", ", $D$1, ", ", $E$1, ", ", $F$1, ", ", $G$1, ", Estado) VALUES(", C30, ", '", D30, "', ", E30, ", '", F30, "', '", G30, "', 1)")</f>
@@ -4404,10 +4426,10 @@
         <v>200</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H31" s="1" t="str">
         <f>_xlfn.CONCAT("INSERT INTO ",Hoja2!$C$8, " (", $C$1, ", ", $D$1, ", ", $E$1, ", ", $F$1, ", ", $G$1, ", Estado) VALUES(", C31, ", '", D31, "', ", E31, ", '", F31, "', '", G31, "', 1)")</f>
@@ -4422,10 +4444,10 @@
         <v>400</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H32" s="1" t="str">
         <f>_xlfn.CONCAT("INSERT INTO ",Hoja2!$C$8, " (", $C$1, ", ", $D$1, ", ", $E$1, ", ", $F$1, ", ", $G$1, ", Estado) VALUES(", C32, ", '", D32, "', ", E32, ", '", F32, "', '", G32, "', 1)")</f>
@@ -4440,10 +4462,10 @@
         <v>444</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H33" s="1" t="str">
         <f>_xlfn.CONCAT("INSERT INTO ",Hoja2!$C$8, " (", $C$1, ", ", $D$1, ", ", $E$1, ", ", $F$1, ", ", $G$1, ", Estado) VALUES(", C33, ", '", D33, "', ", E33, ", '", F33, "', '", G33, "', 1)")</f>
@@ -4458,10 +4480,10 @@
         <v>500</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H34" s="1" t="str">
         <f>_xlfn.CONCAT("INSERT INTO ",Hoja2!$C$8, " (", $C$1, ", ", $D$1, ", ", $E$1, ", ", $F$1, ", ", $G$1, ", Estado) VALUES(", C34, ", '", D34, "', ", E34, ", '", F34, "', '", G34, "', 1)")</f>
@@ -4476,10 +4498,10 @@
         <v>505</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H35" s="1" t="str">
         <f>_xlfn.CONCAT("INSERT INTO ",Hoja2!$C$8, " (", $C$1, ", ", $D$1, ", ", $E$1, ", ", $F$1, ", ", $G$1, ", Estado) VALUES(", C35, ", '", D35, "', ", E35, ", '", F35, "', '", G35, "', 1)")</f>
@@ -4494,10 +4516,10 @@
         <v>508</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H36" s="1" t="str">
         <f>_xlfn.CONCAT("INSERT INTO ",Hoja2!$C$8, " (", $C$1, ", ", $D$1, ", ", $E$1, ", ", $F$1, ", ", $G$1, ", Estado) VALUES(", C36, ", '", D36, "', ", E36, ", '", F36, "', '", G36, "', 1)")</f>
@@ -4512,10 +4534,10 @@
         <v>550</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H37" s="1" t="str">
         <f>_xlfn.CONCAT("INSERT INTO ",Hoja2!$C$8, " (", $C$1, ", ", $D$1, ", ", $E$1, ", ", $F$1, ", ", $G$1, ", Estado) VALUES(", C37, ", '", D37, "', ", E37, ", '", F37, "', '", G37, "', 1)")</f>
@@ -4530,10 +4552,10 @@
         <v>551</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H38" s="1" t="str">
         <f>_xlfn.CONCAT("INSERT INTO ",Hoja2!$C$8, " (", $C$1, ", ", $D$1, ", ", $E$1, ", ", $F$1, ", ", $G$1, ", Estado) VALUES(", C38, ", '", D38, "', ", E38, ", '", F38, "', '", G38, "', 1)")</f>
@@ -4548,10 +4570,10 @@
         <v>552</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H39" s="1" t="str">
         <f>_xlfn.CONCAT("INSERT INTO ",Hoja2!$C$8, " (", $C$1, ", ", $D$1, ", ", $E$1, ", ", $F$1, ", ", $G$1, ", Estado) VALUES(", C39, ", '", D39, "', ", E39, ", '", F39, "', '", G39, "', 1)")</f>
@@ -4566,10 +4588,10 @@
         <v>553</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H40" s="1" t="str">
         <f>_xlfn.CONCAT("INSERT INTO ",Hoja2!$C$8, " (", $C$1, ", ", $D$1, ", ", $E$1, ", ", $F$1, ", ", $G$1, ", Estado) VALUES(", C40, ", '", D40, "', ", E40, ", '", F40, "', '", G40, "', 1)")</f>
@@ -4584,10 +4606,10 @@
         <v>602</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H41" s="1" t="str">
         <f>_xlfn.CONCAT("INSERT INTO ",Hoja2!$C$8, " (", $C$1, ", ", $D$1, ", ", $E$1, ", ", $F$1, ", ", $G$1, ", Estado) VALUES(", C41, ", '", D41, "', ", E41, ", '", F41, "', '", G41, "', 1)")</f>
@@ -4602,10 +4624,10 @@
         <v>701</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H42" s="1" t="str">
         <f>_xlfn.CONCAT("INSERT INTO ",Hoja2!$C$8, " (", $C$1, ", ", $D$1, ", ", $E$1, ", ", $F$1, ", ", $G$1, ", Estado) VALUES(", C42, ", '", D42, "', ", E42, ", '", F42, "', '", G42, "', 1)")</f>
@@ -4620,10 +4642,10 @@
         <v>702</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H43" s="1" t="str">
         <f>_xlfn.CONCAT("INSERT INTO ",Hoja2!$C$8, " (", $C$1, ", ", $D$1, ", ", $E$1, ", ", $F$1, ", ", $G$1, ", Estado) VALUES(", C43, ", '", D43, "', ", E43, ", '", F43, "', '", G43, "', 1)")</f>
@@ -4638,10 +4660,10 @@
         <v>704</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H44" s="1" t="str">
         <f>_xlfn.CONCAT("INSERT INTO ",Hoja2!$C$8, " (", $C$1, ", ", $D$1, ", ", $E$1, ", ", $F$1, ", ", $G$1, ", Estado) VALUES(", C44, ", '", D44, "', ", E44, ", '", F44, "', '", G44, "', 1)")</f>
@@ -4656,10 +4678,10 @@
         <v>705</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H45" s="1" t="str">
         <f>_xlfn.CONCAT("INSERT INTO ",Hoja2!$C$8, " (", $C$1, ", ", $D$1, ", ", $E$1, ", ", $F$1, ", ", $G$1, ", Estado) VALUES(", C45, ", '", D45, "', ", E45, ", '", F45, "', '", G45, "', 1)")</f>
@@ -4674,10 +4696,10 @@
         <v>706</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H46" s="1" t="str">
         <f>_xlfn.CONCAT("INSERT INTO ",Hoja2!$C$8, " (", $C$1, ", ", $D$1, ", ", $E$1, ", ", $F$1, ", ", $G$1, ", Estado) VALUES(", C46, ", '", D46, "', ", E46, ", '", F46, "', '", G46, "', 1)")</f>
@@ -4692,10 +4714,10 @@
         <v>710</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H47" s="1" t="str">
         <f>_xlfn.CONCAT("INSERT INTO ",Hoja2!$C$8, " (", $C$1, ", ", $D$1, ", ", $E$1, ", ", $F$1, ", ", $G$1, ", Estado) VALUES(", C47, ", '", D47, "', ", E47, ", '", F47, "', '", G47, "', 1)")</f>
@@ -4710,10 +4732,10 @@
         <v>711</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H48" s="1" t="str">
         <f>_xlfn.CONCAT("INSERT INTO ",Hoja2!$C$8, " (", $C$1, ", ", $D$1, ", ", $E$1, ", ", $F$1, ", ", $G$1, ", Estado) VALUES(", C48, ", '", D48, "', ", E48, ", '", F48, "', '", G48, "', 1)")</f>
@@ -4728,10 +4750,10 @@
         <v>712</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H49" s="1" t="str">
         <f>_xlfn.CONCAT("INSERT INTO ",Hoja2!$C$8, " (", $C$1, ", ", $D$1, ", ", $E$1, ", ", $F$1, ", ", $G$1, ", Estado) VALUES(", C49, ", '", D49, "', ", E49, ", '", F49, "', '", G49, "', 1)")</f>
@@ -4746,10 +4768,10 @@
         <v>713</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H50" s="1" t="str">
         <f>_xlfn.CONCAT("INSERT INTO ",Hoja2!$C$8, " (", $C$1, ", ", $D$1, ", ", $E$1, ", ", $F$1, ", ", $G$1, ", Estado) VALUES(", C50, ", '", D50, "', ", E50, ", '", F50, "', '", G50, "', 1)")</f>
@@ -4764,10 +4786,10 @@
         <v>714</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H51" s="1" t="str">
         <f>_xlfn.CONCAT("INSERT INTO ",Hoja2!$C$8, " (", $C$1, ", ", $D$1, ", ", $E$1, ", ", $F$1, ", ", $G$1, ", Estado) VALUES(", C51, ", '", D51, "', ", E51, ", '", F51, "', '", G51, "', 1)")</f>
@@ -4782,10 +4804,10 @@
         <v>715</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H52" s="1" t="str">
         <f>_xlfn.CONCAT("INSERT INTO ",Hoja2!$C$8, " (", $C$1, ", ", $D$1, ", ", $E$1, ", ", $F$1, ", ", $G$1, ", Estado) VALUES(", C52, ", '", D52, "', ", E52, ", '", F52, "', '", G52, "', 1)")</f>
@@ -4800,10 +4822,10 @@
         <v>716</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H53" s="1" t="str">
         <f>_xlfn.CONCAT("INSERT INTO ",Hoja2!$C$8, " (", $C$1, ", ", $D$1, ", ", $E$1, ", ", $F$1, ", ", $G$1, ", Estado) VALUES(", C53, ", '", D53, "', ", E53, ", '", F53, "', '", G53, "', 1)")</f>
@@ -4818,10 +4840,10 @@
         <v>717</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H54" s="1" t="str">
         <f>_xlfn.CONCAT("INSERT INTO ",Hoja2!$C$8, " (", $C$1, ", ", $D$1, ", ", $E$1, ", ", $F$1, ", ", $G$1, ", Estado) VALUES(", C54, ", '", D54, "', ", E54, ", '", F54, "', '", G54, "', 1)")</f>
@@ -4836,10 +4858,10 @@
         <v>724</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H55" s="1" t="str">
         <f>_xlfn.CONCAT("INSERT INTO ",Hoja2!$C$8, " (", $C$1, ", ", $D$1, ", ", $E$1, ", ", $F$1, ", ", $G$1, ", Estado) VALUES(", C55, ", '", D55, "', ", E55, ", '", F55, "', '", G55, "', 1)")</f>
@@ -4854,10 +4876,10 @@
         <v>730</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H56" s="1" t="str">
         <f>_xlfn.CONCAT("INSERT INTO ",Hoja2!$C$8, " (", $C$1, ", ", $D$1, ", ", $E$1, ", ", $F$1, ", ", $G$1, ", Estado) VALUES(", C56, ", '", D56, "', ", E56, ", '", F56, "', '", G56, "', 1)")</f>
@@ -4872,10 +4894,10 @@
         <v>788</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H57" s="1" t="str">
         <f>_xlfn.CONCAT("INSERT INTO ",Hoja2!$C$8, " (", $C$1, ", ", $D$1, ", ", $E$1, ", ", $F$1, ", ", $G$1, ", Estado) VALUES(", C57, ", '", D57, "', ", E57, ", '", F57, "', '", G57, "', 1)")</f>
@@ -4890,10 +4912,10 @@
         <v>900</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H58" s="1" t="str">
         <f>_xlfn.CONCAT("INSERT INTO ",Hoja2!$C$8, " (", $C$1, ", ", $D$1, ", ", $E$1, ", ", $F$1, ", ", $G$1, ", Estado) VALUES(", C58, ", '", D58, "', ", E58, ", '", F58, "', '", G58, "', 1)")</f>
@@ -4908,10 +4930,10 @@
         <v>902</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H59" s="1" t="str">
         <f>_xlfn.CONCAT("INSERT INTO ",Hoja2!$C$8, " (", $C$1, ", ", $D$1, ", ", $E$1, ", ", $F$1, ", ", $G$1, ", Estado) VALUES(", C59, ", '", D59, "', ", E59, ", '", F59, "', '", G59, "', 1)")</f>
@@ -4926,7 +4948,7 @@
         <v>12</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H60" s="1" t="str">
         <f>_xlfn.CONCAT("INSERT INTO ",Hoja2!$C$8, " (", $C$1, ", ", $D$1, ", ", $E$1, ", ", $F$1, ", ", $G$1, ", Estado) VALUES(", C60, ", '", D60, "', ", E60, ", '", F60, "', '", G60, "', 1)")</f>
@@ -4941,7 +4963,7 @@
         <v>104</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H61" s="1" t="str">
         <f>_xlfn.CONCAT("INSERT INTO ",Hoja2!$C$8, " (", $C$1, ", ", $D$1, ", ", $E$1, ", ", $F$1, ", ", $G$1, ", Estado) VALUES(", C61, ", '", D61, "', ", E61, ", '", F61, "', '", G61, "', 1)")</f>
@@ -4956,7 +4978,7 @@
         <v>105</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H62" s="1" t="str">
         <f>_xlfn.CONCAT("INSERT INTO ",Hoja2!$C$8, " (", $C$1, ", ", $D$1, ", ", $E$1, ", ", $F$1, ", ", $G$1, ", Estado) VALUES(", C62, ", '", D62, "', ", E62, ", '", F62, "', '", G62, "', 1)")</f>
@@ -4971,7 +4993,7 @@
         <v>335</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H63" s="1" t="str">
         <f>_xlfn.CONCAT("INSERT INTO ",Hoja2!$C$8, " (", $C$1, ", ", $D$1, ", ", $E$1, ", ", $F$1, ", ", $G$1, ", Estado) VALUES(", C63, ", '", D63, "', ", E63, ", '", F63, "', '", G63, "', 1)")</f>
@@ -4986,7 +5008,7 @@
         <v>382</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H64" s="1" t="str">
         <f>_xlfn.CONCAT("INSERT INTO ",Hoja2!$C$8, " (", $C$1, ", ", $D$1, ", ", $E$1, ", ", $F$1, ", ", $G$1, ", Estado) VALUES(", C64, ", '", D64, "', ", E64, ", '", F64, "', '", G64, "', 1)")</f>
@@ -5001,7 +5023,7 @@
         <v>404</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="H65" s="1" t="str">
         <f>_xlfn.CONCAT("INSERT INTO ",Hoja2!$C$8, " (", $C$1, ", ", $D$1, ", ", $E$1, ", ", $F$1, ", ", $G$1, ", Estado) VALUES(", C65, ", '", D65, "', ", E65, ", '", F65, "', '", G65, "', 1)")</f>
@@ -5016,7 +5038,7 @@
         <v>81</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H66" s="1" t="str">
         <f>_xlfn.CONCAT("INSERT INTO ",Hoja2!$C$8, " (", $C$1, ", ", $D$1, ", ", $E$1, ", ", $F$1, ", ", $G$1, ", Estado) VALUES(", C66, ", '", D66, "', ", E66, ", '", F66, "', '", G66, "', 1)")</f>
@@ -5031,7 +5053,7 @@
         <v>417</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H67" s="1" t="str">
         <f>_xlfn.CONCAT("INSERT INTO ",Hoja2!$C$8, " (", $C$1, ", ", $D$1, ", ", $E$1, ", ", $F$1, ", ", $G$1, ", Estado) VALUES(", C67, ", '", D67, "', ", E67, ", '", F67, "', '", G67, "', 1)")</f>
@@ -5046,7 +5068,7 @@
         <v>416</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H68" s="1" t="str">
         <f>_xlfn.CONCAT("INSERT INTO ",Hoja2!$C$8, " (", $C$1, ", ", $D$1, ", ", $E$1, ", ", $F$1, ", ", $G$1, ", Estado) VALUES(", C68, ", '", D68, "', ", E68, ", '", F68, "', '", G68, "', 1)")</f>
@@ -5061,7 +5083,7 @@
         <v>125</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H69" s="1" t="str">
         <f>_xlfn.CONCAT("INSERT INTO ",Hoja2!$C$8, " (", $C$1, ", ", $D$1, ", ", $E$1, ", ", $F$1, ", ", $G$1, ", Estado) VALUES(", C69, ", '", D69, "', ", E69, ", '", F69, "', '", G69, "', 1)")</f>
@@ -5076,10 +5098,10 @@
         <v>12</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H70" s="1" t="str">
         <f>_xlfn.CONCAT("INSERT INTO ",Hoja2!$C$8, " (", $C$1, ", ", $D$1, ", ", $E$1, ", ", $F$1, ", ", $G$1, ", Estado) VALUES(", C70, ", '", D70, "', ", E70, ", '", F70, "', '", G70, "', 1)")</f>
@@ -5094,10 +5116,10 @@
         <v>105</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H71" s="1" t="str">
         <f>_xlfn.CONCAT("INSERT INTO ",Hoja2!$C$8, " (", $C$1, ", ", $D$1, ", ", $E$1, ", ", $F$1, ", ", $G$1, ", Estado) VALUES(", C71, ", '", D71, "', ", E71, ", '", F71, "', '", G71, "', 1)")</f>
@@ -5112,10 +5134,10 @@
         <v>355</v>
       </c>
       <c r="F72" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="G72" s="1" t="s">
         <v>133</v>
-      </c>
-      <c r="G72" s="1" t="s">
-        <v>134</v>
       </c>
       <c r="H72" s="1" t="str">
         <f>_xlfn.CONCAT("INSERT INTO ",Hoja2!$C$8, " (", $C$1, ", ", $D$1, ", ", $E$1, ", ", $F$1, ", ", $G$1, ", Estado) VALUES(", C72, ", '", D72, "', ", E72, ", '", F72, "', '", G72, "', 1)")</f>
@@ -5130,10 +5152,10 @@
         <v>104</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G73" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H73" s="1" t="str">
         <f>_xlfn.CONCAT("INSERT INTO ",Hoja2!$C$8, " (", $C$1, ", ", $D$1, ", ", $E$1, ", ", $F$1, ", ", $G$1, ", Estado) VALUES(", C73, ", '", D73, "', ", E73, ", '", F73, "', '", G73, "', 1)")</f>
@@ -5148,10 +5170,10 @@
         <v>382</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H74" s="1" t="str">
         <f>_xlfn.CONCAT("INSERT INTO ",Hoja2!$C$8, " (", $C$1, ", ", $D$1, ", ", $E$1, ", ", $F$1, ", ", $G$1, ", Estado) VALUES(", C74, ", '", D74, "', ", E74, ", '", F74, "', '", G74, "', 1)")</f>
@@ -5166,10 +5188,10 @@
         <v>404</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G75" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H75" s="1" t="str">
         <f>_xlfn.CONCAT("INSERT INTO ",Hoja2!$C$8, " (", $C$1, ", ", $D$1, ", ", $E$1, ", ", $F$1, ", ", $G$1, ", Estado) VALUES(", C75, ", '", D75, "', ", E75, ", '", F75, "', '", G75, "', 1)")</f>
@@ -5184,10 +5206,10 @@
         <v>81</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H76" s="1" t="str">
         <f>_xlfn.CONCAT("INSERT INTO ",Hoja2!$C$8, " (", $C$1, ", ", $D$1, ", ", $E$1, ", ", $F$1, ", ", $G$1, ", Estado) VALUES(", C76, ", '", D76, "', ", E76, ", '", F76, "', '", G76, "', 1)")</f>
@@ -5202,10 +5224,10 @@
         <v>417</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G77" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H77" s="1" t="str">
         <f>_xlfn.CONCAT("INSERT INTO ",Hoja2!$C$8, " (", $C$1, ", ", $D$1, ", ", $E$1, ", ", $F$1, ", ", $G$1, ", Estado) VALUES(", C77, ", '", D77, "', ", E77, ", '", F77, "', '", G77, "', 1)")</f>
@@ -5220,10 +5242,10 @@
         <v>416</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G78" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H78" s="1" t="str">
         <f>_xlfn.CONCAT("INSERT INTO ",Hoja2!$C$8, " (", $C$1, ", ", $D$1, ", ", $E$1, ", ", $F$1, ", ", $G$1, ", Estado) VALUES(", C78, ", '", D78, "', ", E78, ", '", F78, "', '", G78, "', 1)")</f>
@@ -5238,14 +5260,50 @@
         <v>125</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G79" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H79" s="1" t="str">
         <f>_xlfn.CONCAT("INSERT INTO ",Hoja2!$C$8, " (", $C$1, ", ", $D$1, ", ", $E$1, ", ", $F$1, ", ", $G$1, ", Estado) VALUES(", C79, ", '", D79, "', ", E79, ", '", F79, "', '", G79, "', 1)")</f>
         <v>INSERT INTO TablasDetalles (nIdTabla, Acronimo, Orden, TablaDetalle, Observaciones, Estado) VALUES(7, '', 125, 'dyp_pp_forma_35', 'https://gitlab.sat.gob.mx/avl/[REP]|https://gitlab.sat.gob.mx/avl/[REP]|http://18.144.132.20/proyectos/sat/sdma6/ape1/dyp/[REP]/-/tree/main/Continuidad%20Operativa/Incidencias/RMA-[RMA]/[PAQ]', 1)</v>
+      </c>
+    </row>
+    <row r="80" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C80" s="1">
+        <v>1</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="E80" s="1">
+        <v>0</v>
+      </c>
+      <c r="F80" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="H80" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO ",Hoja2!$C$8, " (", $C$1, ", ", $D$1, ", ", $E$1, ", ", $F$1, ", ", $G$1, ", Estado) VALUES(", C80, ", '", D80, "', ", E80, ", '", F80, "', '", G80, "', 1)")</f>
+        <v>INSERT INTO TablasDetalles (nIdTabla, Acronimo, Orden, TablaDetalle, Observaciones, Estado) VALUES(1, 'MMay', 0, 'Mantenimiento Mayor', '', 1)</v>
+      </c>
+    </row>
+    <row r="81" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C81" s="1">
+        <v>1</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="E81" s="1">
+        <v>0</v>
+      </c>
+      <c r="F81" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H81" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO ",Hoja2!$C$8, " (", $C$1, ", ", $D$1, ", ", $E$1, ", ", $F$1, ", ", $G$1, ", Estado) VALUES(", C81, ", '", D81, "', ", E81, ", '", F81, "', '", G81, "', 1)")</f>
+        <v>INSERT INTO TablasDetalles (nIdTabla, Acronimo, Orden, TablaDetalle, Observaciones, Estado) VALUES(1, 'Servicio', 0, 'Servicio', '', 1)</v>
       </c>
     </row>
   </sheetData>

</xml_diff>